<commit_message>
Added bond conditions and surety, ATN,. ATN sequence and JMS number to Case Initiation
</commit_message>
<xml_diff>
--- a/schemas/CaseInitiation_iepd/artifacts/CaseInitiation_MappingSpreasheet.xlsx
+++ b/schemas/CaseInitiation_iepd/artifacts/CaseInitiation_MappingSpreasheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcp911gov-my.sharepoint.com/personal/aidandelgado_missioncriticalpartners_com/Documents/ONE.WORKSPACE/21. NOLA/EXCHANGES/CASE INITIATION/mappingSpreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\CaseInitiation_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="484" documentId="11_1F25BA0D27419D30275C2A5CEBFB2BAD43792F1F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86BC4C2A-8E9B-4ED6-8B93-CC520835B036}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001C625A-F0D2-4259-8B29-A3EABD10824A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4575" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3390" yWindow="-21315" windowWidth="34395" windowHeight="20535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Case Initiation" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1709" uniqueCount="903">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="929">
   <si>
     <t/>
   </si>
@@ -3268,6 +3268,135 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>MessageOperationCode</t>
+  </si>
+  <si>
+    <t>A type of message operation.</t>
+  </si>
+  <si>
+    <t>nola-ext:UpdateCode</t>
+  </si>
+  <si>
+    <t>structures:MetadataType</t>
+  </si>
+  <si>
+    <t>nola-ext:MessageUpdateCode</t>
+  </si>
+  <si>
+    <t>/nola-ext:UpdateType</t>
+  </si>
+  <si>
+    <t>246</t>
+  </si>
+  <si>
+    <t>Arrest</t>
+  </si>
+  <si>
+    <t>ArrestTrackingNumber</t>
+  </si>
+  <si>
+    <t>The State's Police Automated Fingerprint Inforamtion System (AFIS) generates an ATN to uniquely identify each booking event, often referred to as an Arrest Cycle. The ATN must be communicated from the Sheriff to the Court at a minimum, in order to effectively update the State computerized criminal history (CCH) with dispositions of arrest charges. The ATN is a 12 digit identifier used to track an arrest. ATN is a person-arrest-charge tracking number (combines ATN + ATN Charge Seq #) The ATN is a 12 digit number with an additional 3 digit “charge sequence number”. (Therefore the “15 digit ATN” is unique to Folder#+charge, but the 12 digit ATN is unique only to Folder#.) The 15 digit ATN can be used to track the disposition of each charge associated with a given booking. The Louisiana State Police use a statewide ATN number, but it does not match the ATNs used in Orleans.</t>
+  </si>
+  <si>
+    <t>[{"db": "AS400_JMS",	"table": "IMARRD",	"fieldDesc": "ATN",	"field": "IDATN1"},
+{"db": "AS400_JMS",	"table": "IMARRD",	"fieldDesc": "ATN",	"field": "IDATN2"},
+{"db": "AS400_JMS",	"table": "IMARRD",	"fieldDesc": "ChargeATN",	"field": "IDATN3"},
+{"db": "AS400_JMS",	"table": "IMARRD",	"fieldDesc": "ATN",	"field": "IDATN4"},
+{"db": "AS400_JMS",	"table": "IMARRD",	"fieldDesc": "ChargeATN",	"field": "IDATN5"},
+{"db": "AS400_JMS",	"table": "IMARRD",	"fieldDesc": "ATN",	"field": "IDATN6"},
+{"db": "AS400_JMS",	"table": "IMARRD_ChargesAll_w_Keys",	"fieldDesc": "ATN",	"field": "ATN"},
+{"db": "AS400_JMS",	"table": "IMCHGD",	"fieldDesc": "ATN",	"field": "ICATNO"},
+{"db": "AS400_JMS",	"table": "IMDSPL",	"fieldDesc": "ATN",	"field": "DLATNO"}]</t>
+  </si>
+  <si>
+    <t>nola-ext:StatewideArrestTrackingNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/nola:EntityUpdateExchange/j:Booking/j:Arrest/j:ArrestCharge[1]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
+/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[2]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
+/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[3]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
+/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[4]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
+/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[5]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
+/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[6]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
+</t>
+  </si>
+  <si>
+    <t>247</t>
+  </si>
+  <si>
+    <t>ATNChargeSequenceID</t>
+  </si>
+  <si>
+    <t>A sequential identifier number assigned to the arrest of a subject i.e ATN. The State's Police Automated Fingerprint Inforamtion System (AFIS) generates an ATN to uniquely identify each booking event, often referred to as an Arrest Cycle. The ATN must be communicated from the Sheriff to the Court at a minimum, in order to effectively update the State computerized criminal history (CCH) with dispositions of arrest charges.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[{"db": "AS400_JMS",	"table": "CHRGLOG",	"fieldDesc": "ATNChargeSequenceNumber",	"field": "CXCHRGSEQ"},	
+{"db": "AS400_JMS",	"table": "DEFCHG",	"fieldDesc": "ATNChargeSequenceNumber",	"field": "DCCHRGSEQ"},	
+{"db": "AS400_JMS",	"table": "IMARRD",	"fieldDesc": "ATNChargeSequenceNumber",	"field": "IDATS1"},
+{"db": "AS400_JMS",	"table": "IMARRD",	"fieldDesc": "ATNChargeSequenceNumber",	"field": "IDATS2"},
+{"db": "AS400_JMS",	"table": "IMARRD",	"fieldDesc": "ChargeATNSequenceNumber",	"field": "IDATS3"},
+{"db": "AS400_JMS",	"table": "IMARRD",	"fieldDesc": "ATNChargeSequenceNumber",	"field": "IDATS4"},
+{"db": "AS400_JMS",	"table": "IMARRD",	"fieldDesc": "ChargeATNSequenceNumber",	"field": "IDATS5"},
+{"db": "AS400_JMS",	"table": "IMARRD",	"fieldDesc": "ATNChargeSequenceNumber",	"field": "IDATS6"},	
+{"db": "AS400_JMS",	"table": "IMARRD_ChargesAll_w_Keys",	"fieldDesc": "ATNSequenceNumber",	"field": "ATN_Seq_No"},
+{"db": "AS400_JMS",	"table": "IMCHGD",	"fieldDesc": "ATNSequenceNumber",	"field": "ICATNS"},
+{"db": "AS400_JMS",	"table": "IMDSPL",	"fieldDesc": "ATNChargeSequenceNumber",	"field": "DLATNS"},
+{"db": "AS400_CDC_CMS",	"table": "CHRGLOG",	"fieldDesc": "ATNChargeSequenceNumber",	"field": "CXCHRGSEQ"},
+{"db": "AS400_CDC_CMS",	"table": "DEFCHG",	"fieldDesc": "ATNChargeSequenceNumber",	"field": "DCCHRGSEQ"},
+{"db": "CASTNetDB",	"table": "PersonProbation",	"fieldDesc": "SequenceNumber",	"field": "SequenceNumber"}]
+</t>
+  </si>
+  <si>
+    <t>nola-ext:StatewideATNChargeSequenceID</t>
+  </si>
+  <si>
+    <t>/nola:EntityUpdateExchange/j:Booking/j:Arrest/j:ArrestCharge[1]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
+/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[2]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
+/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[3]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
+/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[4]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
+/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[5]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
+/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[6]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID</t>
+  </si>
+  <si>
+    <t>245</t>
+  </si>
+  <si>
+    <t>FolderNumber</t>
+  </si>
+  <si>
+    <t>A Person ID for single continuous term of incarceration. If the individual is released today and returns tomorrow, a new folder number will be issued.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[{"db": "AS400_JMS",	"table": "IMARRD",	"fieldDesc": "FolderNumber",	"field": "IDFLDR"},
+{"db": "As400_JMS",	"table": "IMEVND",	"fieldDesc": "FolderNumber",	"field": "EDACTV"},
+{"db": "As400_JMS",	"table": "IMFLDR",	"fieldDesc": "FolderNumber",	"field": "IFFLDR"},
+{"db": "As400_JMS",	"table": "IMBPYD",	"fieldDesc": "FolderNumber",	"field": "BDFLDR"},
+{"db": "As400_JMS",	"table": "IMCHGD",	"fieldDesc": "FolderNumber",	"field": "ICFLDR"},
+{"db": "As400_JMS",	"table": "IMDSPL",	"fieldDesc": "FolderNumber",	"field": "DLFLDR"},
+{"db": "As400_JMS",	"table": "IMLOCH",	"fieldDesc": "FolderNumber",	"field": "LHFLDR"},
+{"db": "As400_JMS",	"table": "IMMISC",	"fieldDesc": "FolderNumber",	"field": "MSFLDR"},
+{"db": "As400_JMS",	"table": "IMSMTF",	"fieldDesc": "FolderNumber",	"field": "ISFLDR"},
+{"db": "As400_JMS",	"table": "IMTYPH",	"fieldDesc": "FolderNumber",	"field": "ITFLDR"},
+{"db": "AS400_CDC_CMS",	"table": "DEFCHG",	"fieldDesc": "FolderNumber",	"field": "DCFLDR"},
+{"db": "CASTNetDB",	"table": "ArrestLocation",	"fieldDesc": "FolderNumber",	"field": "FolderNumber"},
+{"db": "CASTNetDB",	"table": "ArrestOfficer",	"fieldDesc": "FolderNumber",	"field": "FolderNumber"},
+{"db": "CASTNetDB",	"table": "PersonArrest",	"fieldDesc": "FolderNumber",	"field": "FolderNumber"},
+{"db": "CASTNetDB",	"table": "ArrestLocation",	"fieldDesc": "FolderNumber",	"field": "FolderNumber"},
+{"db": "CASTNetDB",	"table": "ArrestOfficer",	"fieldDesc": "FolderNumber",	"field": "FolderNumber"},
+{"db": "CASTNetDB",	"table": "PersonArrest",	"fieldDesc": "FolderNumber",	"field": "FolderNumber"},
+{"db": "MC",		"table": "Digicourt_Orleans.dbview.vw_ArrestDetail",	"fieldDesc": "FolderNumber",	"field": "ARREST_FOLDER"}]
+</t>
+  </si>
+  <si>
+    <t>j:BookingDocumentControlIdentification</t>
+  </si>
+  <si>
+    <t>nc:IdentificationType</t>
+  </si>
+  <si>
+    <t>/nola:EntityUpdateExchange/j:Booking/j:BookingDocumentControlIdentification/IdentificationID</t>
   </si>
 </sst>
 </file>
@@ -3296,7 +3425,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3320,8 +3449,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -3381,11 +3516,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3418,6 +3566,18 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3456,54 +3616,6 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -3889,13 +4001,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3909,6 +4014,61 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -3925,22 +4085,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C1555FB-E16C-423D-A1FA-98AD99C9E15B}" name="MappingSpreadsheet" displayName="MappingSpreadsheet" ref="A1:N146" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C1555FB-E16C-423D-A1FA-98AD99C9E15B}" name="MappingSpreadsheet" displayName="MappingSpreadsheet" ref="A1:N146" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="A1:N146" xr:uid="{2C1555FB-E16C-423D-A1FA-98AD99C9E15B}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{A154B48A-3186-466D-92F1-8A6270997FD4}" name="Property Type" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{34D42627-CEA6-4CC6-8595-04D65F5B7FC2}" name="ID" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{AD7378CB-087D-40BA-BF6E-0D2B5B55BA9A}" name="Class" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{36A86CBD-CDD8-44BA-BA43-413750E65A44}" name="Attribute" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{72D45659-5E2F-4BFC-81A5-C5FF4DFE5DDF}" name="Type" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{A3C40E7C-BB7E-4753-B8CA-CFF928923052}" name="Description" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{D2C6663F-C6EC-4594-A9C3-F41EB985C640}" name="Multiplicity" dataDxfId="9"/>
-    <tableColumn id="15" xr3:uid="{D28C8D2A-F576-4E39-A6FD-92022F8631AB}" name="Name" dataDxfId="8"/>
-    <tableColumn id="16" xr3:uid="{074CD765-47FC-4CFC-8E23-CBCE34EC8DBF}" name="&lt;&lt;JTMP_LegacySource&gt;&gt;_x000a_JSON_LegacySourceLocation" dataDxfId="7"/>
-    <tableColumn id="17" xr3:uid="{E5E69126-3108-439D-9E27-7E1133D14689}" name="&lt;&lt;NOLA&gt;&gt;_x000a_NIEM Element" dataDxfId="6"/>
-    <tableColumn id="18" xr3:uid="{8C7A492D-FAF0-4419-91AB-79EFA53429C6}" name="&lt;&lt;NOLA&gt;&gt;_x000a_NIEM Type" dataDxfId="5"/>
-    <tableColumn id="19" xr3:uid="{D0C9BD32-CF2A-4AB2-9BC1-3ABDD5B45D98}" name="&lt;&lt;NOLA&gt;&gt;_x000a_Parent Base Type" dataDxfId="4"/>
-    <tableColumn id="20" xr3:uid="{EE54FF2C-9367-49F7-B18A-E3FBF7B0BEF0}" name="&lt;&lt;NOLA&gt;&gt;_x000a_XPath (relative)" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{A154B48A-3186-466D-92F1-8A6270997FD4}" name="Property Type" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{34D42627-CEA6-4CC6-8595-04D65F5B7FC2}" name="ID" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{AD7378CB-087D-40BA-BF6E-0D2B5B55BA9A}" name="Class" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{36A86CBD-CDD8-44BA-BA43-413750E65A44}" name="Attribute" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{72D45659-5E2F-4BFC-81A5-C5FF4DFE5DDF}" name="Type" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{A3C40E7C-BB7E-4753-B8CA-CFF928923052}" name="Description" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{D2C6663F-C6EC-4594-A9C3-F41EB985C640}" name="Multiplicity" dataDxfId="7"/>
+    <tableColumn id="15" xr3:uid="{D28C8D2A-F576-4E39-A6FD-92022F8631AB}" name="Name" dataDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{074CD765-47FC-4CFC-8E23-CBCE34EC8DBF}" name="&lt;&lt;JTMP_LegacySource&gt;&gt;_x000a_JSON_LegacySourceLocation" dataDxfId="5"/>
+    <tableColumn id="17" xr3:uid="{E5E69126-3108-439D-9E27-7E1133D14689}" name="&lt;&lt;NOLA&gt;&gt;_x000a_NIEM Element" dataDxfId="4"/>
+    <tableColumn id="18" xr3:uid="{8C7A492D-FAF0-4419-91AB-79EFA53429C6}" name="&lt;&lt;NOLA&gt;&gt;_x000a_NIEM Type" dataDxfId="3"/>
+    <tableColumn id="19" xr3:uid="{D0C9BD32-CF2A-4AB2-9BC1-3ABDD5B45D98}" name="&lt;&lt;NOLA&gt;&gt;_x000a_Parent Base Type" dataDxfId="2"/>
+    <tableColumn id="20" xr3:uid="{EE54FF2C-9367-49F7-B18A-E3FBF7B0BEF0}" name="&lt;&lt;NOLA&gt;&gt;_x000a_XPath (relative)" dataDxfId="1"/>
     <tableColumn id="23" xr3:uid="{145A9E88-C30A-482A-BBDC-8D021BDDB1EE}" name="&lt;&lt;NOLA_Exchange&gt;&gt;_x000a_Case Initiation" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4244,31 +4404,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N146"/>
+  <dimension ref="A1:N150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E119" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L140" sqref="L140"/>
+      <selection pane="bottomRight" activeCell="I158" sqref="I158"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" width="15.46484375" customWidth="1"/>
     <col min="2" max="2" width="5" customWidth="1"/>
-    <col min="3" max="3" width="19.44140625" customWidth="1"/>
-    <col min="4" max="4" width="31.88671875" customWidth="1"/>
-    <col min="5" max="5" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="19.46484375" customWidth="1"/>
+    <col min="4" max="4" width="31.86328125" customWidth="1"/>
+    <col min="5" max="5" width="30.1328125" customWidth="1"/>
     <col min="6" max="6" width="35.6640625" customWidth="1"/>
-    <col min="7" max="7" width="13.21875" customWidth="1"/>
+    <col min="7" max="7" width="13.19921875" customWidth="1"/>
     <col min="9" max="9" width="126.33203125" customWidth="1"/>
     <col min="10" max="12" width="11" customWidth="1"/>
-    <col min="13" max="13" width="15.109375" customWidth="1"/>
-    <col min="14" max="14" width="12.77734375" customWidth="1"/>
+    <col min="13" max="13" width="15.1328125" customWidth="1"/>
+    <col min="14" max="14" width="12.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>901</v>
       </c>
@@ -4312,7 +4472,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -4340,7 +4500,7 @@
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
     </row>
-    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
@@ -4382,7 +4542,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="7" t="s">
         <v>12</v>
       </c>
@@ -4424,7 +4584,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -4466,7 +4626,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
@@ -4508,7 +4668,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
@@ -4550,7 +4710,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -4580,7 +4740,7 @@
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
     </row>
-    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="7" t="s">
         <v>12</v>
       </c>
@@ -4622,7 +4782,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="7" t="s">
         <v>12</v>
       </c>
@@ -4664,7 +4824,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -4694,7 +4854,7 @@
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
     </row>
-    <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="7" t="s">
         <v>12</v>
       </c>
@@ -4736,7 +4896,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
@@ -4766,7 +4926,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="7" t="s">
         <v>12</v>
       </c>
@@ -4808,7 +4968,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="7" t="s">
         <v>12</v>
       </c>
@@ -4850,7 +5010,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="7" t="s">
         <v>12</v>
       </c>
@@ -4892,7 +5052,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="7" t="s">
         <v>12</v>
       </c>
@@ -4934,7 +5094,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="7" t="s">
         <v>12</v>
       </c>
@@ -4976,7 +5136,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="7" t="s">
         <v>12</v>
       </c>
@@ -5018,7 +5178,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="7" t="s">
         <v>12</v>
       </c>
@@ -5060,7 +5220,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="7" t="s">
         <v>12</v>
       </c>
@@ -5102,7 +5262,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="7" t="s">
         <v>12</v>
       </c>
@@ -5144,7 +5304,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="7" t="s">
         <v>12</v>
       </c>
@@ -5186,7 +5346,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>8</v>
       </c>
@@ -5214,7 +5374,7 @@
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
     </row>
-    <row r="25" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="11" t="s">
         <v>410</v>
       </c>
@@ -5250,7 +5410,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="7" t="s">
         <v>12</v>
       </c>
@@ -5292,7 +5452,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="7" t="s">
         <v>12</v>
       </c>
@@ -5334,7 +5494,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>8</v>
       </c>
@@ -5362,7 +5522,7 @@
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
     </row>
-    <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>8</v>
       </c>
@@ -5390,7 +5550,7 @@
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
     </row>
-    <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="7" t="s">
         <v>12</v>
       </c>
@@ -5432,7 +5592,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="7" t="s">
         <v>12</v>
       </c>
@@ -5474,7 +5634,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="11" t="s">
         <v>410</v>
       </c>
@@ -5512,7 +5672,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="11" t="s">
         <v>410</v>
       </c>
@@ -5552,7 +5712,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="7" t="s">
         <v>12</v>
       </c>
@@ -5594,7 +5754,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="7" t="s">
         <v>12</v>
       </c>
@@ -5634,7 +5794,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="7" t="s">
         <v>12</v>
       </c>
@@ -5676,7 +5836,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="7" t="s">
         <v>12</v>
       </c>
@@ -5720,7 +5880,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="7" t="s">
         <v>12</v>
       </c>
@@ -5764,7 +5924,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="7" t="s">
         <v>12</v>
       </c>
@@ -5806,7 +5966,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="7" t="s">
         <v>12</v>
       </c>
@@ -5848,7 +6008,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="7" t="s">
         <v>12</v>
       </c>
@@ -5890,7 +6050,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="7" t="s">
         <v>12</v>
       </c>
@@ -5932,7 +6092,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="7" t="s">
         <v>12</v>
       </c>
@@ -5974,7 +6134,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="7" t="s">
         <v>12</v>
       </c>
@@ -6018,7 +6178,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="11" t="s">
         <v>410</v>
       </c>
@@ -6058,7 +6218,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="7" t="s">
         <v>12</v>
       </c>
@@ -6100,7 +6260,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="7" t="s">
         <v>12</v>
       </c>
@@ -6142,7 +6302,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="7" t="s">
         <v>12</v>
       </c>
@@ -6186,7 +6346,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="7" t="s">
         <v>12</v>
       </c>
@@ -6230,7 +6390,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="3" t="s">
         <v>8</v>
       </c>
@@ -6264,7 +6424,7 @@
       </c>
       <c r="N50" s="4"/>
     </row>
-    <row r="51" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="7" t="s">
         <v>12</v>
       </c>
@@ -6306,7 +6466,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="7" t="s">
         <v>12</v>
       </c>
@@ -6348,7 +6508,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="7" t="s">
         <v>12</v>
       </c>
@@ -6390,7 +6550,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="11" t="s">
         <v>410</v>
       </c>
@@ -6426,7 +6586,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="7" t="s">
         <v>12</v>
       </c>
@@ -6470,7 +6630,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="7" t="s">
         <v>12</v>
       </c>
@@ -6514,7 +6674,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="7" t="s">
         <v>12</v>
       </c>
@@ -6558,7 +6718,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="7" t="s">
         <v>12</v>
       </c>
@@ -6600,7 +6760,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="7" t="s">
         <v>12</v>
       </c>
@@ -6642,7 +6802,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="3" t="s">
         <v>8</v>
       </c>
@@ -6678,7 +6838,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="11" t="s">
         <v>410</v>
       </c>
@@ -6712,7 +6872,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A62" s="7" t="s">
         <v>12</v>
       </c>
@@ -6754,7 +6914,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="7" t="s">
         <v>12</v>
       </c>
@@ -6796,7 +6956,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="7" t="s">
         <v>12</v>
       </c>
@@ -6838,7 +6998,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65" s="11" t="s">
         <v>410</v>
       </c>
@@ -6878,7 +7038,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="7" t="s">
         <v>12</v>
       </c>
@@ -6922,7 +7082,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="11" t="s">
         <v>410</v>
       </c>
@@ -6958,7 +7118,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="7" t="s">
         <v>12</v>
       </c>
@@ -7002,7 +7162,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="7" t="s">
         <v>12</v>
       </c>
@@ -7044,7 +7204,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="7" t="s">
         <v>12</v>
       </c>
@@ -7088,7 +7248,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="11" t="s">
         <v>410</v>
       </c>
@@ -7126,7 +7286,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A72" s="7" t="s">
         <v>12</v>
       </c>
@@ -7168,7 +7328,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="7" t="s">
         <v>12</v>
       </c>
@@ -7210,7 +7370,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="11" t="s">
         <v>410</v>
       </c>
@@ -7246,7 +7406,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75" s="7" t="s">
         <v>12</v>
       </c>
@@ -7282,7 +7442,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76" s="7" t="s">
         <v>12</v>
       </c>
@@ -7318,7 +7478,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="7" t="s">
         <v>12</v>
       </c>
@@ -7360,7 +7520,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="7" t="s">
         <v>12</v>
       </c>
@@ -7400,7 +7560,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79" s="7" t="s">
         <v>12</v>
       </c>
@@ -7436,7 +7596,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A80" s="3" t="s">
         <v>8</v>
       </c>
@@ -7468,7 +7628,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81" s="7" t="s">
         <v>12</v>
       </c>
@@ -7510,7 +7670,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="3" t="s">
         <v>8</v>
       </c>
@@ -7546,7 +7706,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A83" s="7" t="s">
         <v>12</v>
       </c>
@@ -7590,7 +7750,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A84" s="7" t="s">
         <v>12</v>
       </c>
@@ -7632,7 +7792,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A85" s="7" t="s">
         <v>12</v>
       </c>
@@ -7674,7 +7834,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A86" s="7" t="s">
         <v>12</v>
       </c>
@@ -7716,7 +7876,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A87" s="3" t="s">
         <v>8</v>
       </c>
@@ -7750,7 +7910,7 @@
       </c>
       <c r="N87" s="4"/>
     </row>
-    <row r="88" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A88" s="7" t="s">
         <v>12</v>
       </c>
@@ -7792,7 +7952,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="89" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A89" s="7" t="s">
         <v>12</v>
       </c>
@@ -7834,7 +7994,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A90" s="7" t="s">
         <v>12</v>
       </c>
@@ -7878,7 +8038,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A91" s="7" t="s">
         <v>12</v>
       </c>
@@ -7922,7 +8082,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A92" s="11" t="s">
         <v>410</v>
       </c>
@@ -7960,7 +8120,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A93" s="3" t="s">
         <v>8</v>
       </c>
@@ -7992,7 +8152,7 @@
       </c>
       <c r="N93" s="4"/>
     </row>
-    <row r="94" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A94" s="7" t="s">
         <v>12</v>
       </c>
@@ -8034,7 +8194,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A95" s="7" t="s">
         <v>12</v>
       </c>
@@ -8076,7 +8236,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A96" s="11" t="s">
         <v>410</v>
       </c>
@@ -8116,7 +8276,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A97" s="3" t="s">
         <v>8</v>
       </c>
@@ -8144,7 +8304,7 @@
       <c r="M97" s="4"/>
       <c r="N97" s="4"/>
     </row>
-    <row r="98" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A98" s="7" t="s">
         <v>12</v>
       </c>
@@ -8186,7 +8346,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A99" s="7" t="s">
         <v>12</v>
       </c>
@@ -8228,7 +8388,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A100" s="3" t="s">
         <v>8</v>
       </c>
@@ -8260,7 +8420,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A101" s="3" t="s">
         <v>8</v>
       </c>
@@ -8290,7 +8450,7 @@
       <c r="M101" s="4"/>
       <c r="N101" s="4"/>
     </row>
-    <row r="102" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A102" s="7" t="s">
         <v>12</v>
       </c>
@@ -8332,7 +8492,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A103" s="7" t="s">
         <v>12</v>
       </c>
@@ -8374,7 +8534,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="104" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A104" s="3" t="s">
         <v>8</v>
       </c>
@@ -8408,7 +8568,7 @@
       </c>
       <c r="N104" s="4"/>
     </row>
-    <row r="105" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A105" s="3" t="s">
         <v>8</v>
       </c>
@@ -8438,7 +8598,7 @@
       </c>
       <c r="N105" s="4"/>
     </row>
-    <row r="106" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A106" s="7" t="s">
         <v>12</v>
       </c>
@@ -8480,7 +8640,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A107" s="7" t="s">
         <v>12</v>
       </c>
@@ -8522,7 +8682,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A108" s="7" t="s">
         <v>12</v>
       </c>
@@ -8564,7 +8724,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A109" s="7" t="s">
         <v>12</v>
       </c>
@@ -8606,7 +8766,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A110" s="3" t="s">
         <v>8</v>
       </c>
@@ -8636,7 +8796,7 @@
       <c r="M110" s="4"/>
       <c r="N110" s="4"/>
     </row>
-    <row r="111" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A111" s="3" t="s">
         <v>8</v>
       </c>
@@ -8666,7 +8826,7 @@
       <c r="M111" s="4"/>
       <c r="N111" s="4"/>
     </row>
-    <row r="112" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A112" s="7" t="s">
         <v>12</v>
       </c>
@@ -8708,7 +8868,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A113" s="3" t="s">
         <v>8</v>
       </c>
@@ -8734,7 +8894,7 @@
       <c r="M113" s="4"/>
       <c r="N113" s="4"/>
     </row>
-    <row r="114" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A114" s="7" t="s">
         <v>12</v>
       </c>
@@ -8774,7 +8934,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="115" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A115" s="7" t="s">
         <v>12</v>
       </c>
@@ -8816,7 +8976,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="116" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A116" s="7" t="s">
         <v>12</v>
       </c>
@@ -8858,7 +9018,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="117" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A117" s="3" t="s">
         <v>8</v>
       </c>
@@ -8886,7 +9046,7 @@
       <c r="M117" s="4"/>
       <c r="N117" s="4"/>
     </row>
-    <row r="118" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A118" s="11" t="s">
         <v>410</v>
       </c>
@@ -8926,7 +9086,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A119" s="11" t="s">
         <v>410</v>
       </c>
@@ -8966,7 +9126,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A120" s="11" t="s">
         <v>410</v>
       </c>
@@ -9006,7 +9166,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="121" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A121" s="3" t="s">
         <v>8</v>
       </c>
@@ -9034,7 +9194,7 @@
       <c r="M121" s="4"/>
       <c r="N121" s="4"/>
     </row>
-    <row r="122" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A122" s="7" t="s">
         <v>12</v>
       </c>
@@ -9076,7 +9236,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="123" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A123" s="7" t="s">
         <v>12</v>
       </c>
@@ -9118,7 +9278,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="124" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A124" s="7" t="s">
         <v>12</v>
       </c>
@@ -9160,7 +9320,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="125" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A125" s="3" t="s">
         <v>8</v>
       </c>
@@ -9188,7 +9348,7 @@
       <c r="M125" s="4"/>
       <c r="N125" s="4"/>
     </row>
-    <row r="126" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A126" s="7" t="s">
         <v>12</v>
       </c>
@@ -9230,7 +9390,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="127" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A127" s="7" t="s">
         <v>12</v>
       </c>
@@ -9270,7 +9430,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="128" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A128" s="7" t="s">
         <v>12</v>
       </c>
@@ -9312,7 +9472,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="129" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A129" s="7" t="s">
         <v>12</v>
       </c>
@@ -9354,7 +9514,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="130" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A130" s="3" t="s">
         <v>8</v>
       </c>
@@ -9388,7 +9548,7 @@
       </c>
       <c r="N130" s="4"/>
     </row>
-    <row r="131" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A131" s="7" t="s">
         <v>12</v>
       </c>
@@ -9430,7 +9590,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="132" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A132" s="7" t="s">
         <v>12</v>
       </c>
@@ -9472,7 +9632,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="133" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A133" s="7" t="s">
         <v>12</v>
       </c>
@@ -9514,7 +9674,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="134" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A134" s="7" t="s">
         <v>12</v>
       </c>
@@ -9556,7 +9716,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="135" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A135" s="7" t="s">
         <v>12</v>
       </c>
@@ -9598,7 +9758,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="136" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A136" s="3" t="s">
         <v>8</v>
       </c>
@@ -9626,7 +9786,7 @@
       <c r="M136" s="4"/>
       <c r="N136" s="4"/>
     </row>
-    <row r="137" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A137" s="7" t="s">
         <v>12</v>
       </c>
@@ -9668,7 +9828,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="138" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A138" s="7" t="s">
         <v>12</v>
       </c>
@@ -9710,7 +9870,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="139" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A139" s="7" t="s">
         <v>12</v>
       </c>
@@ -9752,7 +9912,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="140" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A140" s="7" t="s">
         <v>12</v>
       </c>
@@ -9794,7 +9954,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="141" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A141" s="7" t="s">
         <v>12</v>
       </c>
@@ -9836,7 +9996,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="142" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A142" s="3" t="s">
         <v>8</v>
       </c>
@@ -9866,7 +10026,7 @@
       <c r="M142" s="4"/>
       <c r="N142" s="4"/>
     </row>
-    <row r="143" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A143" s="7" t="s">
         <v>12</v>
       </c>
@@ -9908,7 +10068,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="144" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A144" s="3" t="s">
         <v>8</v>
       </c>
@@ -9938,7 +10098,7 @@
       <c r="M144" s="4"/>
       <c r="N144" s="4"/>
     </row>
-    <row r="145" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A145" s="7" t="s">
         <v>12</v>
       </c>
@@ -9980,7 +10140,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="146" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A146" s="7" t="s">
         <v>12</v>
       </c>
@@ -10020,6 +10180,166 @@
       </c>
       <c r="N146" s="9" t="s">
         <v>469</v>
+      </c>
+    </row>
+    <row r="147" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A147" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B147" s="13"/>
+      <c r="C147" s="13"/>
+      <c r="D147" s="14" t="s">
+        <v>903</v>
+      </c>
+      <c r="E147" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F147" s="14" t="s">
+        <v>904</v>
+      </c>
+      <c r="G147" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="H147" s="13"/>
+      <c r="I147" s="13"/>
+      <c r="J147" s="13" t="s">
+        <v>905</v>
+      </c>
+      <c r="K147" s="13" t="s">
+        <v>906</v>
+      </c>
+      <c r="L147" s="13"/>
+      <c r="M147" s="13" t="s">
+        <v>907</v>
+      </c>
+      <c r="N147" s="13" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="148" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A148" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B148" s="15" t="s">
+        <v>909</v>
+      </c>
+      <c r="C148" s="15" t="s">
+        <v>910</v>
+      </c>
+      <c r="D148" s="15" t="s">
+        <v>911</v>
+      </c>
+      <c r="E148" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F148" s="15" t="s">
+        <v>912</v>
+      </c>
+      <c r="G148" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="H148" s="15" t="s">
+        <v>911</v>
+      </c>
+      <c r="I148" s="15" t="s">
+        <v>913</v>
+      </c>
+      <c r="J148" s="15" t="s">
+        <v>913</v>
+      </c>
+      <c r="K148" s="15" t="s">
+        <v>914</v>
+      </c>
+      <c r="L148" s="15" t="s">
+        <v>456</v>
+      </c>
+      <c r="M148" s="15"/>
+      <c r="N148" s="15" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="149" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A149" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B149" s="15" t="s">
+        <v>916</v>
+      </c>
+      <c r="C149" s="15" t="s">
+        <v>910</v>
+      </c>
+      <c r="D149" s="15" t="s">
+        <v>917</v>
+      </c>
+      <c r="E149" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F149" s="15" t="s">
+        <v>918</v>
+      </c>
+      <c r="G149" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="H149" s="15" t="s">
+        <v>917</v>
+      </c>
+      <c r="I149" s="15" t="s">
+        <v>919</v>
+      </c>
+      <c r="J149" s="15" t="s">
+        <v>919</v>
+      </c>
+      <c r="K149" s="15" t="s">
+        <v>920</v>
+      </c>
+      <c r="L149" s="15" t="s">
+        <v>456</v>
+      </c>
+      <c r="M149" s="15"/>
+      <c r="N149" s="15" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="150" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A150" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B150" s="15" t="s">
+        <v>922</v>
+      </c>
+      <c r="C150" s="15" t="s">
+        <v>910</v>
+      </c>
+      <c r="D150" s="15" t="s">
+        <v>923</v>
+      </c>
+      <c r="E150" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F150" s="15" t="s">
+        <v>924</v>
+      </c>
+      <c r="G150" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H150" s="15" t="s">
+        <v>923</v>
+      </c>
+      <c r="I150" s="15" t="s">
+        <v>925</v>
+      </c>
+      <c r="J150" s="15" t="s">
+        <v>925</v>
+      </c>
+      <c r="K150" s="15" t="s">
+        <v>926</v>
+      </c>
+      <c r="L150" s="15" t="s">
+        <v>927</v>
+      </c>
+      <c r="M150" s="15"/>
+      <c r="N150" s="15" t="s">
+        <v>928</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed XPath for several recently added booking elements in the CaseInitiation mapping document; updated the example
</commit_message>
<xml_diff>
--- a/schemas/CaseInitiation_iepd/artifacts/CaseInitiation_MappingSpreasheet.xlsx
+++ b/schemas/CaseInitiation_iepd/artifacts/CaseInitiation_MappingSpreasheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\CaseInitiation_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0002F1-5DA8-4591-8481-A5E4CACF954E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E0128A-2E12-426E-B174-2C89C08FE5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4065" yWindow="-21600" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4080" yWindow="-21720" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Case Initiation" sheetId="1" r:id="rId1"/>
@@ -3314,15 +3314,6 @@
     <t>nola-ext:StatewideArrestTrackingNumber</t>
   </si>
   <si>
-    <t xml:space="preserve">/nola:EntityUpdateExchange/j:Booking/j:Arrest/j:ArrestCharge[1]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
-/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[2]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
-/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[3]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
-/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[4]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
-/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[5]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
-/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[6]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
-</t>
-  </si>
-  <si>
     <t>247</t>
   </si>
   <si>
@@ -3350,14 +3341,6 @@
   </si>
   <si>
     <t>nola-ext:StatewideATNChargeSequenceID</t>
-  </si>
-  <si>
-    <t>/nola:EntityUpdateExchange/j:Booking/j:Arrest/j:ArrestCharge[1]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
-/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[2]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
-/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[3]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
-/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[4]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
-/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[5]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
-/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[6]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID</t>
   </si>
   <si>
     <t>245</t>
@@ -3396,9 +3379,6 @@
     <t>nc:IdentificationType</t>
   </si>
   <si>
-    <t>/nola:EntityUpdateExchange/j:Booking/j:BookingDocumentControlIdentification/IdentificationID</t>
-  </si>
-  <si>
     <t xml:space="preserve">/j:Booking/j:Arrest/j:ArrestCharge[1]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
 /nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[2]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
 /nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[3]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
@@ -3417,6 +3397,26 @@
   </si>
   <si>
     <t>/j:Booking/j:BookingDocumentControlIdentification/IdentificationID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/nola:CaseInitiationExchange/CourtCase/j:CaseAugmentation/j:CaseCharge/j:ChargeSubject/j:SubjectBooking/j:Arrest/j:ArrestCharge[1]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
+/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[2]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
+/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[3]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
+/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[4]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
+/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[5]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
+/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[6]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
+</t>
+  </si>
+  <si>
+    <t>/nola:CaseInitiationExchange/CourtCase/j:CaseAugmentation/j:CaseCharge/j:ChargeSubject/j:SubjectBooking/j:Arrest/j:ArrestCharge[1]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
+/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[2]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
+/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[3]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
+/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[4]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
+/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[5]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
+/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[6]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID</t>
+  </si>
+  <si>
+    <t>/nola:CaseInitiationExchange/CourtCase/j:CaseAugmentation/j:CaseCharge/j:ChargeSubject/j:SubjectBooking/j:BookingDocumentControlIdentification/IdentificationID</t>
   </si>
 </sst>
 </file>
@@ -4428,10 +4428,10 @@
   <dimension ref="A1:N150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E110" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E137" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D147" sqref="D147"/>
+      <selection pane="bottomRight" activeCell="N162" sqref="N162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -4446,7 +4446,7 @@
     <col min="9" max="9" width="126.33203125" customWidth="1"/>
     <col min="10" max="12" width="11" customWidth="1"/>
     <col min="13" max="13" width="15.1328125" customWidth="1"/>
-    <col min="14" max="14" width="12.796875" customWidth="1"/>
+    <col min="14" max="14" width="106.9296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.45">
@@ -10273,10 +10273,10 @@
       </c>
       <c r="L148" s="16"/>
       <c r="M148" s="15" t="s">
+        <v>926</v>
+      </c>
+      <c r="N148" s="15" t="s">
         <v>929</v>
-      </c>
-      <c r="N148" s="15" t="s">
-        <v>915</v>
       </c>
     </row>
     <row r="149" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10284,41 +10284,41 @@
         <v>12</v>
       </c>
       <c r="B149" s="15" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="C149" s="15" t="s">
         <v>910</v>
       </c>
       <c r="D149" s="15" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="E149" s="15" t="s">
         <v>65</v>
       </c>
       <c r="F149" s="15" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="G149" s="15" t="s">
         <v>36</v>
       </c>
       <c r="H149" s="15" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="I149" s="15" t="s">
+        <v>918</v>
+      </c>
+      <c r="J149" s="15" t="s">
         <v>919</v>
-      </c>
-      <c r="J149" s="15" t="s">
-        <v>920</v>
       </c>
       <c r="K149" s="15" t="s">
         <v>456</v>
       </c>
       <c r="L149" s="16"/>
       <c r="M149" s="15" t="s">
+        <v>927</v>
+      </c>
+      <c r="N149" s="15" t="s">
         <v>930</v>
-      </c>
-      <c r="N149" s="15" t="s">
-        <v>921</v>
       </c>
     </row>
     <row r="150" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10326,41 +10326,41 @@
         <v>12</v>
       </c>
       <c r="B150" s="15" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="C150" s="15" t="s">
         <v>910</v>
       </c>
       <c r="D150" s="15" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="E150" s="15" t="s">
         <v>13</v>
       </c>
       <c r="F150" s="15" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="G150" s="15" t="s">
         <v>14</v>
       </c>
       <c r="H150" s="15" t="s">
+        <v>921</v>
+      </c>
+      <c r="I150" s="15" t="s">
         <v>923</v>
       </c>
-      <c r="I150" s="15" t="s">
+      <c r="J150" s="15" t="s">
+        <v>924</v>
+      </c>
+      <c r="K150" s="15" t="s">
         <v>925</v>
-      </c>
-      <c r="J150" s="15" t="s">
-        <v>926</v>
-      </c>
-      <c r="K150" s="15" t="s">
-        <v>927</v>
       </c>
       <c r="L150" s="16"/>
       <c r="M150" s="15" t="s">
+        <v>928</v>
+      </c>
+      <c r="N150" s="15" t="s">
         <v>931</v>
-      </c>
-      <c r="N150" s="15" t="s">
-        <v>928</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed [1]s in XPaths in the CaseInitiation mapping
</commit_message>
<xml_diff>
--- a/schemas/CaseInitiation_iepd/artifacts/CaseInitiation_MappingSpreasheet.xlsx
+++ b/schemas/CaseInitiation_iepd/artifacts/CaseInitiation_MappingSpreasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\CaseInitiation_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E0128A-2E12-426E-B174-2C89C08FE5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4166FB5D-43D8-4C07-8284-9DCD5C1E794D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4080" yWindow="-21720" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4080" yWindow="-21720" windowWidth="51840" windowHeight="20760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Case Initiation" sheetId="1" r:id="rId1"/>
@@ -2798,11 +2798,6 @@
     <t>[{"db": "AS400_CDC_CMS",	"table": "CHRGLOG",	"fieldDesc": "EffectiveDate",	"field": "CXEDATE"}]</t>
   </si>
   <si>
-    <t xml:space="preserve">/j:ArrestCharge[1]/j:ChargeFilingDate/DateTime
-/j:CaseCharge/j:ChargeFilingDate/DateTime
-</t>
-  </si>
-  <si>
     <t>/nola:CaseInitiationExchange/CourtCase/j:CaseAugmentation/j:CaseCharge/j:ChargeFilingDate/DateTime</t>
   </si>
   <si>
@@ -3379,7 +3374,18 @@
     <t>nc:IdentificationType</t>
   </si>
   <si>
-    <t xml:space="preserve">/j:Booking/j:Arrest/j:ArrestCharge[1]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
+    <t>/j:Booking/j:BookingDocumentControlIdentification/IdentificationID</t>
+  </si>
+  <si>
+    <t>/nola:CaseInitiationExchange/CourtCase/j:CaseAugmentation/j:CaseCharge/j:ChargeSubject/j:SubjectBooking/j:BookingDocumentControlIdentification/IdentificationID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/j:ArrestCharge/j:ChargeFilingDate/DateTime
+/j:CaseCharge/j:ChargeFilingDate/DateTime
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/j:Booking/j:Arrest/j:ArrestCharge/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
 /nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[2]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
 /nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[3]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
 /nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[4]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
@@ -3388,18 +3394,7 @@
 </t>
   </si>
   <si>
-    <t>/j:Booking/j:Arrest/j:ArrestCharge[1]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
-/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[2]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
-/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[3]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
-/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[4]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
-/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[5]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
-/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[6]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID</t>
-  </si>
-  <si>
-    <t>/j:Booking/j:BookingDocumentControlIdentification/IdentificationID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/nola:CaseInitiationExchange/CourtCase/j:CaseAugmentation/j:CaseCharge/j:ChargeSubject/j:SubjectBooking/j:Arrest/j:ArrestCharge[1]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
+    <t xml:space="preserve">/nola:CaseInitiationExchange/CourtCase/j:CaseAugmentation/j:CaseCharge/j:ChargeSubject/j:SubjectBooking/j:Arrest/j:ArrestCharge/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
 /nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[2]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
 /nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[3]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
 /nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[4]/nola-ext:ChargeAugmentation/nola-ext:StatewideArrestTrackingNumber
@@ -3408,7 +3403,7 @@
 </t>
   </si>
   <si>
-    <t>/nola:CaseInitiationExchange/CourtCase/j:CaseAugmentation/j:CaseCharge/j:ChargeSubject/j:SubjectBooking/j:Arrest/j:ArrestCharge[1]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
+    <t>/j:Booking/j:Arrest/j:ArrestCharge/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
 /nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[2]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
 /nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[3]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
 /nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[4]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
@@ -3416,7 +3411,12 @@
 /nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[6]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID</t>
   </si>
   <si>
-    <t>/nola:CaseInitiationExchange/CourtCase/j:CaseAugmentation/j:CaseCharge/j:ChargeSubject/j:SubjectBooking/j:BookingDocumentControlIdentification/IdentificationID</t>
+    <t>/nola:CaseInitiationExchange/CourtCase/j:CaseAugmentation/j:CaseCharge/j:ChargeSubject/j:SubjectBooking/j:Arrest/j:ArrestCharge/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
+/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[2]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
+/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[3]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
+/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[4]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
+/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[5]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
+/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[6]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID</t>
   </si>
 </sst>
 </file>
@@ -4428,10 +4428,10 @@
   <dimension ref="A1:N150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E137" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E123" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N162" sqref="N162"/>
+      <selection pane="bottomRight" activeCell="M149" sqref="M149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -4451,7 +4451,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -4504,7 +4504,7 @@
         <v>161</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="4" t="s">
@@ -4742,7 +4742,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="4" t="s">
@@ -4856,7 +4856,7 @@
         <v>90</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="4" t="s">
@@ -4928,7 +4928,7 @@
         <v>226</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="4" t="s">
@@ -5378,7 +5378,7 @@
         <v>288</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="4" t="s">
@@ -5425,10 +5425,10 @@
       <c r="K25" s="9"/>
       <c r="L25" s="9"/>
       <c r="M25" s="9" t="s">
+        <v>886</v>
+      </c>
+      <c r="N25" s="9" t="s">
         <v>887</v>
-      </c>
-      <c r="N25" s="9" t="s">
-        <v>888</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5526,7 +5526,7 @@
         <v>68</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
@@ -5554,7 +5554,7 @@
         <v>328</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="4" t="s">
@@ -5680,17 +5680,17 @@
       <c r="H32" s="9"/>
       <c r="I32" s="9"/>
       <c r="J32" s="9" t="s">
+        <v>866</v>
+      </c>
+      <c r="K32" s="9" t="s">
         <v>867</v>
-      </c>
-      <c r="K32" s="9" t="s">
-        <v>868</v>
       </c>
       <c r="L32" s="9"/>
       <c r="M32" s="9" t="s">
+        <v>868</v>
+      </c>
+      <c r="N32" s="9" t="s">
         <v>869</v>
-      </c>
-      <c r="N32" s="9" t="s">
-        <v>870</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5717,20 +5717,20 @@
       </c>
       <c r="H33" s="9"/>
       <c r="I33" s="9" t="s">
+        <v>870</v>
+      </c>
+      <c r="J33" s="9" t="s">
         <v>871</v>
       </c>
-      <c r="J33" s="9" t="s">
+      <c r="K33" s="9" t="s">
         <v>872</v>
-      </c>
-      <c r="K33" s="9" t="s">
-        <v>873</v>
       </c>
       <c r="L33" s="9"/>
       <c r="M33" s="9" t="s">
+        <v>873</v>
+      </c>
+      <c r="N33" s="9" t="s">
         <v>874</v>
-      </c>
-      <c r="N33" s="9" t="s">
-        <v>875</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5759,20 +5759,20 @@
         <v>358</v>
       </c>
       <c r="I34" s="9" t="s">
+        <v>803</v>
+      </c>
+      <c r="J34" s="9" t="s">
         <v>804</v>
-      </c>
-      <c r="J34" s="9" t="s">
-        <v>805</v>
       </c>
       <c r="K34" s="9" t="s">
         <v>461</v>
       </c>
       <c r="L34" s="9"/>
       <c r="M34" s="9" t="s">
+        <v>805</v>
+      </c>
+      <c r="N34" s="9" t="s">
         <v>806</v>
-      </c>
-      <c r="N34" s="9" t="s">
-        <v>807</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5801,10 +5801,10 @@
         <v>379</v>
       </c>
       <c r="I35" s="9" t="s">
+        <v>831</v>
+      </c>
+      <c r="J35" s="9" t="s">
         <v>832</v>
-      </c>
-      <c r="J35" s="9" t="s">
-        <v>833</v>
       </c>
       <c r="K35" s="9" t="s">
         <v>461</v>
@@ -5812,7 +5812,7 @@
       <c r="L35" s="9"/>
       <c r="M35" s="9"/>
       <c r="N35" s="9" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5939,10 +5939,10 @@
         <v>0</v>
       </c>
       <c r="M38" s="9" t="s">
+        <v>927</v>
+      </c>
+      <c r="N38" s="9" t="s">
         <v>786</v>
-      </c>
-      <c r="N38" s="9" t="s">
-        <v>787</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5971,20 +5971,20 @@
         <v>370</v>
       </c>
       <c r="I39" s="9" t="s">
+        <v>818</v>
+      </c>
+      <c r="J39" s="9" t="s">
         <v>819</v>
-      </c>
-      <c r="J39" s="9" t="s">
-        <v>820</v>
       </c>
       <c r="K39" s="9" t="s">
         <v>461</v>
       </c>
       <c r="L39" s="9"/>
       <c r="M39" s="9" t="s">
+        <v>820</v>
+      </c>
+      <c r="N39" s="9" t="s">
         <v>821</v>
-      </c>
-      <c r="N39" s="9" t="s">
-        <v>822</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6013,20 +6013,20 @@
         <v>346</v>
       </c>
       <c r="I40" s="9" t="s">
+        <v>787</v>
+      </c>
+      <c r="J40" s="9" t="s">
         <v>788</v>
-      </c>
-      <c r="J40" s="9" t="s">
-        <v>789</v>
       </c>
       <c r="K40" s="9" t="s">
         <v>456</v>
       </c>
       <c r="L40" s="9"/>
       <c r="M40" s="9" t="s">
+        <v>789</v>
+      </c>
+      <c r="N40" s="9" t="s">
         <v>790</v>
-      </c>
-      <c r="N40" s="9" t="s">
-        <v>791</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6055,20 +6055,20 @@
         <v>349</v>
       </c>
       <c r="I41" s="9" t="s">
+        <v>791</v>
+      </c>
+      <c r="J41" s="9" t="s">
         <v>792</v>
-      </c>
-      <c r="J41" s="9" t="s">
-        <v>793</v>
       </c>
       <c r="K41" s="9" t="s">
         <v>456</v>
       </c>
       <c r="L41" s="9"/>
       <c r="M41" s="9" t="s">
+        <v>793</v>
+      </c>
+      <c r="N41" s="9" t="s">
         <v>794</v>
-      </c>
-      <c r="N41" s="9" t="s">
-        <v>795</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6097,20 +6097,20 @@
         <v>352</v>
       </c>
       <c r="I42" s="9" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="J42" s="9" t="s">
         <v>455</v>
       </c>
       <c r="K42" s="9" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="L42" s="9"/>
       <c r="M42" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="N42" s="9" t="s">
         <v>798</v>
-      </c>
-      <c r="N42" s="9" t="s">
-        <v>799</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6139,20 +6139,20 @@
         <v>355</v>
       </c>
       <c r="I43" s="9" t="s">
+        <v>799</v>
+      </c>
+      <c r="J43" s="9" t="s">
         <v>800</v>
-      </c>
-      <c r="J43" s="9" t="s">
-        <v>801</v>
       </c>
       <c r="K43" s="9" t="s">
         <v>456</v>
       </c>
       <c r="L43" s="9"/>
       <c r="M43" s="9" t="s">
+        <v>801</v>
+      </c>
+      <c r="N43" s="9" t="s">
         <v>802</v>
-      </c>
-      <c r="N43" s="9" t="s">
-        <v>803</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6181,10 +6181,10 @@
         <v>364</v>
       </c>
       <c r="I44" s="9" t="s">
+        <v>810</v>
+      </c>
+      <c r="J44" s="9" t="s">
         <v>811</v>
-      </c>
-      <c r="J44" s="9" t="s">
-        <v>812</v>
       </c>
       <c r="K44" s="9" t="s">
         <v>461</v>
@@ -6193,10 +6193,10 @@
         <v>0</v>
       </c>
       <c r="M44" s="9" t="s">
+        <v>812</v>
+      </c>
+      <c r="N44" s="9" t="s">
         <v>813</v>
-      </c>
-      <c r="N44" s="9" t="s">
-        <v>814</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6226,17 +6226,17 @@
       </c>
       <c r="I45" s="9"/>
       <c r="J45" s="9" t="s">
+        <v>878</v>
+      </c>
+      <c r="K45" s="9" t="s">
         <v>879</v>
-      </c>
-      <c r="K45" s="9" t="s">
-        <v>880</v>
       </c>
       <c r="L45" s="9"/>
       <c r="M45" s="9" t="s">
+        <v>880</v>
+      </c>
+      <c r="N45" s="9" t="s">
         <v>881</v>
-      </c>
-      <c r="N45" s="9" t="s">
-        <v>882</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6265,20 +6265,20 @@
         <v>361</v>
       </c>
       <c r="I46" s="9" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="J46" s="9" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="K46" s="9" t="s">
         <v>461</v>
       </c>
       <c r="L46" s="9"/>
       <c r="M46" s="9" t="s">
+        <v>808</v>
+      </c>
+      <c r="N46" s="9" t="s">
         <v>809</v>
-      </c>
-      <c r="N46" s="9" t="s">
-        <v>810</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6307,20 +6307,20 @@
         <v>367</v>
       </c>
       <c r="I47" s="9" t="s">
+        <v>814</v>
+      </c>
+      <c r="J47" s="9" t="s">
         <v>815</v>
-      </c>
-      <c r="J47" s="9" t="s">
-        <v>816</v>
       </c>
       <c r="K47" s="9" t="s">
         <v>461</v>
       </c>
       <c r="L47" s="9"/>
       <c r="M47" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="N47" s="9" t="s">
         <v>817</v>
-      </c>
-      <c r="N47" s="9" t="s">
-        <v>818</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6349,10 +6349,10 @@
         <v>373</v>
       </c>
       <c r="I48" s="9" t="s">
+        <v>822</v>
+      </c>
+      <c r="J48" s="9" t="s">
         <v>823</v>
-      </c>
-      <c r="J48" s="9" t="s">
-        <v>824</v>
       </c>
       <c r="K48" s="9" t="s">
         <v>461</v>
@@ -6361,10 +6361,10 @@
         <v>0</v>
       </c>
       <c r="M48" s="9" t="s">
+        <v>824</v>
+      </c>
+      <c r="N48" s="9" t="s">
         <v>825</v>
-      </c>
-      <c r="N48" s="9" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6393,22 +6393,22 @@
         <v>376</v>
       </c>
       <c r="I49" s="9" t="s">
+        <v>826</v>
+      </c>
+      <c r="J49" s="9" t="s">
         <v>827</v>
       </c>
-      <c r="J49" s="9" t="s">
+      <c r="K49" s="9" t="s">
         <v>828</v>
-      </c>
-      <c r="K49" s="9" t="s">
-        <v>829</v>
       </c>
       <c r="L49" s="9" t="s">
         <v>0</v>
       </c>
       <c r="M49" s="9" t="s">
+        <v>829</v>
+      </c>
+      <c r="N49" s="9" t="s">
         <v>830</v>
-      </c>
-      <c r="N49" s="9" t="s">
-        <v>831</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6422,7 +6422,7 @@
         <v>261</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E50" s="5"/>
       <c r="F50" s="4" t="s">
@@ -6596,15 +6596,15 @@
       <c r="H54" s="9"/>
       <c r="I54" s="9"/>
       <c r="J54" s="9" t="s">
+        <v>875</v>
+      </c>
+      <c r="K54" s="9" t="s">
         <v>876</v>
-      </c>
-      <c r="K54" s="9" t="s">
-        <v>877</v>
       </c>
       <c r="L54" s="9"/>
       <c r="M54" s="9"/>
       <c r="N54" s="9" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6834,7 +6834,7 @@
         <v>179</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E60" s="5"/>
       <c r="F60" s="4" t="s">
@@ -6887,10 +6887,10 @@
       <c r="K61" s="9"/>
       <c r="L61" s="9"/>
       <c r="M61" s="9" t="s">
+        <v>892</v>
+      </c>
+      <c r="N61" s="9" t="s">
         <v>893</v>
-      </c>
-      <c r="N61" s="9" t="s">
-        <v>894</v>
       </c>
     </row>
     <row r="62" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7046,17 +7046,17 @@
       </c>
       <c r="I65" s="9"/>
       <c r="J65" s="9" t="s">
+        <v>894</v>
+      </c>
+      <c r="K65" s="9" t="s">
         <v>895</v>
-      </c>
-      <c r="K65" s="9" t="s">
-        <v>896</v>
       </c>
       <c r="L65" s="9"/>
       <c r="M65" s="9" t="s">
+        <v>896</v>
+      </c>
+      <c r="N65" s="9" t="s">
         <v>897</v>
-      </c>
-      <c r="N65" s="9" t="s">
-        <v>898</v>
       </c>
     </row>
     <row r="66" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7128,15 +7128,15 @@
       <c r="H67" s="9"/>
       <c r="I67" s="9"/>
       <c r="J67" s="9" t="s">
+        <v>889</v>
+      </c>
+      <c r="K67" s="9" t="s">
         <v>890</v>
-      </c>
-      <c r="K67" s="9" t="s">
-        <v>891</v>
       </c>
       <c r="L67" s="9"/>
       <c r="M67" s="9"/>
       <c r="N67" s="9" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="68" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7304,7 +7304,7 @@
         <v>566</v>
       </c>
       <c r="N71" s="9" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="72" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7416,7 +7416,7 @@
       <c r="H74" s="9"/>
       <c r="I74" s="9"/>
       <c r="J74" s="9" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="K74" s="9" t="s">
         <v>538</v>
@@ -7424,7 +7424,7 @@
       <c r="L74" s="9"/>
       <c r="M74" s="9"/>
       <c r="N74" s="9" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="75" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7628,7 +7628,7 @@
         <v>46</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E80" s="5"/>
       <c r="F80" s="4" t="s">
@@ -7702,7 +7702,7 @@
         <v>117</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E82" s="5"/>
       <c r="F82" s="4" t="s">
@@ -7908,7 +7908,7 @@
         <v>135</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E87" s="5"/>
       <c r="F87" s="4" t="s">
@@ -8126,19 +8126,19 @@
       <c r="H92" s="9"/>
       <c r="I92" s="9"/>
       <c r="J92" s="9" t="s">
+        <v>882</v>
+      </c>
+      <c r="K92" s="9" t="s">
         <v>883</v>
       </c>
-      <c r="K92" s="9" t="s">
+      <c r="L92" s="9" t="s">
         <v>884</v>
-      </c>
-      <c r="L92" s="9" t="s">
-        <v>885</v>
       </c>
       <c r="M92" s="9" t="s">
         <v>483</v>
       </c>
       <c r="N92" s="9" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="93" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8152,7 +8152,7 @@
         <v>318</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E93" s="5"/>
       <c r="F93" s="4" t="s">
@@ -8284,17 +8284,17 @@
       </c>
       <c r="I96" s="9"/>
       <c r="J96" s="9" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="K96" s="9" t="s">
         <v>769</v>
       </c>
       <c r="L96" s="9"/>
       <c r="M96" s="9" t="s">
+        <v>859</v>
+      </c>
+      <c r="N96" s="9" t="s">
         <v>860</v>
-      </c>
-      <c r="N96" s="9" t="s">
-        <v>861</v>
       </c>
     </row>
     <row r="97" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8308,7 +8308,7 @@
         <v>151</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E97" s="5"/>
       <c r="F97" s="4" t="s">
@@ -8420,7 +8420,7 @@
         <v>315</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E100" s="5"/>
       <c r="F100" s="4" t="s">
@@ -8452,7 +8452,7 @@
         <v>96</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E101" s="5"/>
       <c r="F101" s="4" t="s">
@@ -8566,7 +8566,7 @@
         <v>132</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E104" s="5"/>
       <c r="F104" s="4" t="s">
@@ -8600,7 +8600,7 @@
         <v>52</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E105" s="5"/>
       <c r="F105" s="4" t="s">
@@ -8798,7 +8798,7 @@
         <v>70</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E110" s="5"/>
       <c r="F110" s="4" t="s">
@@ -8828,7 +8828,7 @@
         <v>38</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E111" s="5"/>
       <c r="F111" s="4" t="s">
@@ -8900,7 +8900,7 @@
         <v>105</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E113" s="5"/>
       <c r="F113" s="5"/>
@@ -9050,7 +9050,7 @@
         <v>408</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E117" s="5"/>
       <c r="F117" s="4" t="s">
@@ -9097,14 +9097,14 @@
         <v>645</v>
       </c>
       <c r="K118" s="9" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="L118" s="9"/>
       <c r="M118" s="9" t="s">
+        <v>861</v>
+      </c>
+      <c r="N118" s="9" t="s">
         <v>862</v>
-      </c>
-      <c r="N118" s="9" t="s">
-        <v>863</v>
       </c>
     </row>
     <row r="119" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9141,10 +9141,10 @@
       </c>
       <c r="L119" s="9"/>
       <c r="M119" s="9" t="s">
+        <v>861</v>
+      </c>
+      <c r="N119" s="9" t="s">
         <v>862</v>
-      </c>
-      <c r="N119" s="9" t="s">
-        <v>863</v>
       </c>
     </row>
     <row r="120" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9181,10 +9181,10 @@
       </c>
       <c r="L120" s="9"/>
       <c r="M120" s="9" t="s">
+        <v>864</v>
+      </c>
+      <c r="N120" s="9" t="s">
         <v>865</v>
-      </c>
-      <c r="N120" s="9" t="s">
-        <v>866</v>
       </c>
     </row>
     <row r="121" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9198,7 +9198,7 @@
         <v>382</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E121" s="5"/>
       <c r="F121" s="4" t="s">
@@ -9241,20 +9241,20 @@
         <v>388</v>
       </c>
       <c r="I122" s="9" t="s">
+        <v>838</v>
+      </c>
+      <c r="J122" s="9" t="s">
         <v>839</v>
-      </c>
-      <c r="J122" s="9" t="s">
-        <v>840</v>
       </c>
       <c r="K122" s="9" t="s">
         <v>461</v>
       </c>
       <c r="L122" s="9"/>
       <c r="M122" s="9" t="s">
+        <v>840</v>
+      </c>
+      <c r="N122" s="9" t="s">
         <v>841</v>
-      </c>
-      <c r="N122" s="9" t="s">
-        <v>842</v>
       </c>
     </row>
     <row r="123" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9283,20 +9283,20 @@
         <v>386</v>
       </c>
       <c r="I123" s="9" t="s">
+        <v>834</v>
+      </c>
+      <c r="J123" s="9" t="s">
         <v>835</v>
-      </c>
-      <c r="J123" s="9" t="s">
-        <v>836</v>
       </c>
       <c r="K123" s="9" t="s">
         <v>461</v>
       </c>
       <c r="L123" s="9"/>
       <c r="M123" s="9" t="s">
+        <v>836</v>
+      </c>
+      <c r="N123" s="9" t="s">
         <v>837</v>
-      </c>
-      <c r="N123" s="9" t="s">
-        <v>838</v>
       </c>
     </row>
     <row r="124" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9325,20 +9325,20 @@
         <v>391</v>
       </c>
       <c r="I124" s="9" t="s">
+        <v>842</v>
+      </c>
+      <c r="J124" s="9" t="s">
         <v>843</v>
-      </c>
-      <c r="J124" s="9" t="s">
-        <v>844</v>
       </c>
       <c r="K124" s="9" t="s">
         <v>604</v>
       </c>
       <c r="L124" s="9"/>
       <c r="M124" s="9" t="s">
+        <v>844</v>
+      </c>
+      <c r="N124" s="9" t="s">
         <v>845</v>
-      </c>
-      <c r="N124" s="9" t="s">
-        <v>846</v>
       </c>
     </row>
     <row r="125" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9352,7 +9352,7 @@
         <v>394</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E125" s="5"/>
       <c r="F125" s="4" t="s">
@@ -9395,7 +9395,7 @@
         <v>397</v>
       </c>
       <c r="I126" s="9" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="J126" s="9" t="s">
         <v>666</v>
@@ -9405,10 +9405,10 @@
       </c>
       <c r="L126" s="9"/>
       <c r="M126" s="9" t="s">
+        <v>847</v>
+      </c>
+      <c r="N126" s="9" t="s">
         <v>848</v>
-      </c>
-      <c r="N126" s="9" t="s">
-        <v>849</v>
       </c>
     </row>
     <row r="127" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9438,17 +9438,17 @@
       </c>
       <c r="I127" s="9"/>
       <c r="J127" s="9" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="K127" s="9" t="s">
         <v>456</v>
       </c>
       <c r="L127" s="9"/>
       <c r="M127" s="9" t="s">
+        <v>856</v>
+      </c>
+      <c r="N127" s="9" t="s">
         <v>857</v>
-      </c>
-      <c r="N127" s="9" t="s">
-        <v>858</v>
       </c>
     </row>
     <row r="128" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9477,7 +9477,7 @@
         <v>400</v>
       </c>
       <c r="I128" s="9" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="J128" s="9" t="s">
         <v>455</v>
@@ -9487,10 +9487,10 @@
       </c>
       <c r="L128" s="9"/>
       <c r="M128" s="9" t="s">
+        <v>850</v>
+      </c>
+      <c r="N128" s="9" t="s">
         <v>851</v>
-      </c>
-      <c r="N128" s="9" t="s">
-        <v>852</v>
       </c>
     </row>
     <row r="129" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9519,7 +9519,7 @@
         <v>403</v>
       </c>
       <c r="I129" s="9" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="J129" s="9" t="s">
         <v>455</v>
@@ -9529,10 +9529,10 @@
       </c>
       <c r="L129" s="9"/>
       <c r="M129" s="9" t="s">
+        <v>853</v>
+      </c>
+      <c r="N129" s="9" t="s">
         <v>854</v>
-      </c>
-      <c r="N129" s="9" t="s">
-        <v>855</v>
       </c>
     </row>
     <row r="130" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9546,7 +9546,7 @@
         <v>297</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E130" s="5"/>
       <c r="F130" s="4" t="s">
@@ -9790,7 +9790,7 @@
         <v>73</v>
       </c>
       <c r="D136" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E136" s="5"/>
       <c r="F136" s="4" t="s">
@@ -10028,7 +10028,7 @@
         <v>31</v>
       </c>
       <c r="D142" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E142" s="5"/>
       <c r="F142" s="4" t="s">
@@ -10100,7 +10100,7 @@
         <v>22</v>
       </c>
       <c r="D144" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E144" s="5"/>
       <c r="F144" s="4" t="s">
@@ -10210,13 +10210,13 @@
       <c r="B147" s="13"/>
       <c r="C147" s="13"/>
       <c r="D147" s="14" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="E147" s="14" t="s">
         <v>13</v>
       </c>
       <c r="F147" s="14" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="G147" s="14" t="s">
         <v>36</v>
@@ -10224,17 +10224,17 @@
       <c r="H147" s="13"/>
       <c r="I147" s="13"/>
       <c r="J147" s="13" t="s">
+        <v>904</v>
+      </c>
+      <c r="K147" s="13" t="s">
         <v>905</v>
-      </c>
-      <c r="K147" s="13" t="s">
-        <v>906</v>
       </c>
       <c r="L147" s="13"/>
       <c r="M147" s="13" t="s">
+        <v>906</v>
+      </c>
+      <c r="N147" s="13" t="s">
         <v>907</v>
-      </c>
-      <c r="N147" s="13" t="s">
-        <v>908</v>
       </c>
     </row>
     <row r="148" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10242,38 +10242,38 @@
         <v>12</v>
       </c>
       <c r="B148" s="15" t="s">
+        <v>908</v>
+      </c>
+      <c r="C148" s="15" t="s">
         <v>909</v>
       </c>
-      <c r="C148" s="15" t="s">
+      <c r="D148" s="15" t="s">
         <v>910</v>
-      </c>
-      <c r="D148" s="15" t="s">
-        <v>911</v>
       </c>
       <c r="E148" s="15" t="s">
         <v>13</v>
       </c>
       <c r="F148" s="15" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="G148" s="15" t="s">
         <v>36</v>
       </c>
       <c r="H148" s="15" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="I148" s="15" t="s">
+        <v>912</v>
+      </c>
+      <c r="J148" s="15" t="s">
         <v>913</v>
-      </c>
-      <c r="J148" s="15" t="s">
-        <v>914</v>
       </c>
       <c r="K148" s="15" t="s">
         <v>456</v>
       </c>
       <c r="L148" s="16"/>
       <c r="M148" s="15" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="N148" s="15" t="s">
         <v>929</v>
@@ -10284,41 +10284,41 @@
         <v>12</v>
       </c>
       <c r="B149" s="15" t="s">
+        <v>914</v>
+      </c>
+      <c r="C149" s="15" t="s">
+        <v>909</v>
+      </c>
+      <c r="D149" s="15" t="s">
         <v>915</v>
-      </c>
-      <c r="C149" s="15" t="s">
-        <v>910</v>
-      </c>
-      <c r="D149" s="15" t="s">
-        <v>916</v>
       </c>
       <c r="E149" s="15" t="s">
         <v>65</v>
       </c>
       <c r="F149" s="15" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="G149" s="15" t="s">
         <v>36</v>
       </c>
       <c r="H149" s="15" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="I149" s="15" t="s">
+        <v>917</v>
+      </c>
+      <c r="J149" s="15" t="s">
         <v>918</v>
-      </c>
-      <c r="J149" s="15" t="s">
-        <v>919</v>
       </c>
       <c r="K149" s="15" t="s">
         <v>456</v>
       </c>
       <c r="L149" s="16"/>
       <c r="M149" s="15" t="s">
-        <v>927</v>
+        <v>930</v>
       </c>
       <c r="N149" s="15" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
     </row>
     <row r="150" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10326,41 +10326,41 @@
         <v>12</v>
       </c>
       <c r="B150" s="15" t="s">
+        <v>919</v>
+      </c>
+      <c r="C150" s="15" t="s">
+        <v>909</v>
+      </c>
+      <c r="D150" s="15" t="s">
         <v>920</v>
-      </c>
-      <c r="C150" s="15" t="s">
-        <v>910</v>
-      </c>
-      <c r="D150" s="15" t="s">
-        <v>921</v>
       </c>
       <c r="E150" s="15" t="s">
         <v>13</v>
       </c>
       <c r="F150" s="15" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="G150" s="15" t="s">
         <v>14</v>
       </c>
       <c r="H150" s="15" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="I150" s="15" t="s">
+        <v>922</v>
+      </c>
+      <c r="J150" s="15" t="s">
         <v>923</v>
       </c>
-      <c r="J150" s="15" t="s">
+      <c r="K150" s="15" t="s">
         <v>924</v>
-      </c>
-      <c r="K150" s="15" t="s">
-        <v>925</v>
       </c>
       <c r="L150" s="16"/>
       <c r="M150" s="15" t="s">
-        <v>928</v>
+        <v>925</v>
       </c>
       <c r="N150" s="15" t="s">
-        <v>931</v>
+        <v>926</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Victim/Witness contact information to CaseInitiation and EntityUpdate exchanges
</commit_message>
<xml_diff>
--- a/schemas/CaseInitiation_iepd/artifacts/CaseInitiation_MappingSpreasheet.xlsx
+++ b/schemas/CaseInitiation_iepd/artifacts/CaseInitiation_MappingSpreasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\CaseInitiation_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4166FB5D-43D8-4C07-8284-9DCD5C1E794D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3528B720-2977-48B7-9E02-6529A164F5DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4080" yWindow="-21720" windowWidth="51840" windowHeight="20760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="932">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1794" uniqueCount="951">
   <si>
     <t/>
   </si>
@@ -3418,12 +3418,75 @@
 /nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[5]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
 /nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[6]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID</t>
   </si>
+  <si>
+    <t>EmailAddress</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>ContactAddress</t>
+  </si>
+  <si>
+    <t>A physical location at which a person may be contacted.</t>
+  </si>
+  <si>
+    <t>nc:ContactMailingAddress</t>
+  </si>
+  <si>
+    <t>nc:AddressType</t>
+  </si>
+  <si>
+    <t>nc:ContactInformationType</t>
+  </si>
+  <si>
+    <t>/nc:RoleOfPerson/nc:PersonContactInformation/nc:ContactMailingAddress/</t>
+  </si>
+  <si>
+    <t>An email address by which a case party will be notified electronically.</t>
+  </si>
+  <si>
+    <t>A data concept for a telephone number.</t>
+  </si>
+  <si>
+    <t>nc:ContactEmailID</t>
+  </si>
+  <si>
+    <t>nc:ContactTelephoneNumber</t>
+  </si>
+  <si>
+    <t>/nola:CaseInitiationExchange/CourtCase/j:CaseAugmentation/j:CaseCharge/j:ChargeVictim/RoleOfPerson/nc:PersonContactInformation/nc:ContactMailingAddress</t>
+  </si>
+  <si>
+    <t>/nc:RoleOfPerson/nc:PersonContactInformation/nc:ContactEmailID</t>
+  </si>
+  <si>
+    <t>/nc:RoleOfPerson/nc:PersonContactInformation/nc:ContactTelephoneNumber</t>
+  </si>
+  <si>
+    <t>nc:TelephoneNumberType</t>
+  </si>
+  <si>
+    <t>[{"db": "AS400_JMS",	"table": "IMARRD",	"fieldDesc": "Witness1PhoneNumber",	"field": "IDPHONW1"},
+{"db": "AS400_JMS",	"table": "IMARRD",	"fieldDesc": "Witness2PhoneNumber",	"field": "IDPHONW2"},
+{"db": "AS400_JMS",	"table": "IMMSTR",	"fieldDesc": "PhoneNumber",	"field": "IMPHNO"},
+{"db": "AS400_JMS",	"table": "IMFLDR",	"fieldDesc": "PhoneNumber",	"field": "IFPHNO"},
+{"db": "AS400_CDC_CMS","table": "DEFEND",	"fieldDesc": "PhoneNumber",	"field": "DEFONE"},
+{"db": "EPR",		"table": "VictimPersons",	"fieldDesc": "PhoneNumber",	"field": "PhoneNumber"},
+{"db": "EPR",		"table": "VictimPersons",	"fieldDesc": "WorkPhoneNumber",	"field": "WorkPhoneNumber"}]</t>
+  </si>
+  <si>
+    <t>/nola:CaseInitiationExchange/CourtCase/j:CaseAugmentation/j:CaseCharge/j:ChargeVictim/RoleOfPerson/nc:PersonContactInformation/nc:ContactEmailID</t>
+  </si>
+  <si>
+    <t>/nola:CaseInitiationExchange/CourtCase/j:CaseAugmentation/j:CaseCharge/j:ChargeVictim/RoleOfPerson/nc:PersonContactInformation/nc:ContactTelephoneNumber/</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -3443,6 +3506,12 @@
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -3476,7 +3545,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -3549,11 +3618,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3601,6 +3690,15 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4425,13 +4523,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N150"/>
+  <dimension ref="A1:N153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E123" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E131" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M149" sqref="M149"/>
+      <selection pane="bottomRight" activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -10363,11 +10461,140 @@
         <v>926</v>
       </c>
     </row>
+    <row r="151" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A151" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B151" s="19">
+        <v>357</v>
+      </c>
+      <c r="C151" s="18" t="s">
+        <v>408</v>
+      </c>
+      <c r="D151" s="18" t="s">
+        <v>934</v>
+      </c>
+      <c r="E151" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F151" s="18" t="s">
+        <v>935</v>
+      </c>
+      <c r="G151" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H151" s="18" t="s">
+        <v>934</v>
+      </c>
+      <c r="I151" s="16"/>
+      <c r="J151" s="18" t="s">
+        <v>936</v>
+      </c>
+      <c r="K151" s="18" t="s">
+        <v>937</v>
+      </c>
+      <c r="L151" s="16" t="s">
+        <v>938</v>
+      </c>
+      <c r="M151" s="18" t="s">
+        <v>939</v>
+      </c>
+      <c r="N151" s="18" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A152" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B152" s="19">
+        <v>358</v>
+      </c>
+      <c r="C152" s="18" t="s">
+        <v>408</v>
+      </c>
+      <c r="D152" s="18" t="s">
+        <v>932</v>
+      </c>
+      <c r="E152" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F152" s="18" t="s">
+        <v>940</v>
+      </c>
+      <c r="G152" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H152" s="18" t="s">
+        <v>932</v>
+      </c>
+      <c r="I152" s="16"/>
+      <c r="J152" s="18" t="s">
+        <v>942</v>
+      </c>
+      <c r="K152" s="18" t="s">
+        <v>456</v>
+      </c>
+      <c r="L152" s="16" t="s">
+        <v>938</v>
+      </c>
+      <c r="M152" s="16" t="s">
+        <v>945</v>
+      </c>
+      <c r="N152" s="18" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="153" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A153" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B153" s="19">
+        <v>359</v>
+      </c>
+      <c r="C153" s="18" t="s">
+        <v>408</v>
+      </c>
+      <c r="D153" s="18" t="s">
+        <v>933</v>
+      </c>
+      <c r="E153" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F153" s="18" t="s">
+        <v>941</v>
+      </c>
+      <c r="G153" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H153" s="18" t="s">
+        <v>933</v>
+      </c>
+      <c r="I153" s="18" t="s">
+        <v>948</v>
+      </c>
+      <c r="J153" s="18" t="s">
+        <v>943</v>
+      </c>
+      <c r="K153" s="18" t="s">
+        <v>947</v>
+      </c>
+      <c r="L153" s="16" t="s">
+        <v>938</v>
+      </c>
+      <c r="M153" s="16" t="s">
+        <v>946</v>
+      </c>
+      <c r="N153" s="18" t="s">
+        <v>950</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O147">
     <sortCondition ref="C2:C147"/>
     <sortCondition ref="D2:D147"/>
   </sortState>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Added DispositionDescriptionText to ChargeDisposition
</commit_message>
<xml_diff>
--- a/schemas/CaseInitiation_iepd/artifacts/CaseInitiation_MappingSpreasheet.xlsx
+++ b/schemas/CaseInitiation_iepd/artifacts/CaseInitiation_MappingSpreasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\CaseInitiation_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF47388-C615-4A1D-BF19-D48584FA9C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A054E6F-5E32-4215-B081-C4185188196A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4080" yWindow="-21720" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Case Initiation" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1820" uniqueCount="964">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="971">
   <si>
     <t/>
   </si>
@@ -3084,9 +3084,6 @@
 {"db": "EPR",		"table": "VictimPersons",	"fieldDesc": "WorkPhoneNumber",	"field": "WorkPhoneNumber"}]</t>
   </si>
   <si>
-    <t>ChargeDisposiotion</t>
-  </si>
-  <si>
     <t>ChargeDispositionCode</t>
   </si>
   <si>
@@ -3531,6 +3528,32 @@
   </si>
   <si>
     <t>/nola:CaseInitiationExchange/nc:CourtCase/j:CaseAugmentation/j:CaseCharge/j:ChargeDisposition/nc:DispositionDate/nc:Date</t>
+  </si>
+  <si>
+    <t>ChargeDisposition</t>
+  </si>
+  <si>
+    <t>DispositionDescription</t>
+  </si>
+  <si>
+    <t>A description of a disposition.</t>
+  </si>
+  <si>
+    <t>[{"db": "AS400_CDC_CMS",	"table": "TABDSP",	"fieldDesc": "DispositionDescription",	"field": "DT_DISPOSITION_DESCRIPTION"},
+{"db": "AS400_CDC_CMS",	"table": "TABDSPext",	"fieldDesc": "DispositionDescription",	"field": "DT_DISPOSITION_DESCRIPTION"},
+{"db": "MC",	"table": "Digicourt_Orleans.dbview.vw_CriminalCaseFileDetail",	"fieldDesc": "Disposition",	"field": "disposition"}]</t>
+  </si>
+  <si>
+    <t>nc:DispositionDescriptionText</t>
+  </si>
+  <si>
+    <t>j:CaseCharge/j:ChargeDisposition/nc:DispositionDate/nc:Date</t>
+  </si>
+  <si>
+    <t>j:CaseCharge/j:ChargeDisposition/nc:DispositionDescriptionText</t>
+  </si>
+  <si>
+    <t>nc:DispositionType</t>
   </si>
 </sst>
 </file>
@@ -3717,7 +3740,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3783,10 +3806,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -4700,13 +4719,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V155"/>
+  <dimension ref="A1:V156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E128" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E137" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N155" sqref="A154:N155"/>
+      <selection pane="bottomRight" activeCell="N156" sqref="A154:N156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -4835,7 +4854,7 @@
         <v>561</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -4877,7 +4896,7 @@
         <v>563</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -4919,7 +4938,7 @@
         <v>566</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -4961,7 +4980,7 @@
         <v>570</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5003,7 +5022,7 @@
         <v>573</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5075,7 +5094,7 @@
         <v>461</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5117,7 +5136,7 @@
         <v>457</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5189,7 +5208,7 @@
         <v>504</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5219,7 +5238,7 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5261,7 +5280,7 @@
         <v>606</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5303,7 +5322,7 @@
         <v>609</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5345,7 +5364,7 @@
         <v>613</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5387,7 +5406,7 @@
         <v>615</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5429,7 +5448,7 @@
         <v>617</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5471,7 +5490,7 @@
         <v>620</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5513,7 +5532,7 @@
         <v>623</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5555,7 +5574,7 @@
         <v>626</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5597,7 +5616,7 @@
         <v>629</v>
       </c>
       <c r="N22" s="9" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5639,7 +5658,7 @@
         <v>632</v>
       </c>
       <c r="N23" s="9" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5703,7 +5722,7 @@
         <v>773</v>
       </c>
       <c r="N25" s="9" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5745,7 +5764,7 @@
         <v>659</v>
       </c>
       <c r="N26" s="9" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5787,7 +5806,7 @@
         <v>661</v>
       </c>
       <c r="N27" s="9" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5885,7 +5904,7 @@
         <v>693</v>
       </c>
       <c r="N30" s="9" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5927,7 +5946,7 @@
         <v>0</v>
       </c>
       <c r="N31" s="9" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5965,7 +5984,7 @@
         <v>760</v>
       </c>
       <c r="N32" s="9" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6005,7 +6024,7 @@
         <v>764</v>
       </c>
       <c r="N33" s="9" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6047,7 +6066,7 @@
         <v>715</v>
       </c>
       <c r="N34" s="9" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6087,7 +6106,7 @@
       <c r="L35" s="9"/>
       <c r="M35" s="9"/>
       <c r="N35" s="9" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6129,7 +6148,7 @@
         <v>697</v>
       </c>
       <c r="N36" s="9" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6173,7 +6192,7 @@
         <v>699</v>
       </c>
       <c r="N37" s="9" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6217,7 +6236,7 @@
         <v>807</v>
       </c>
       <c r="N38" s="9" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6259,7 +6278,7 @@
         <v>726</v>
       </c>
       <c r="N39" s="9" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6301,7 +6320,7 @@
         <v>703</v>
       </c>
       <c r="N40" s="9" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6343,7 +6362,7 @@
         <v>706</v>
       </c>
       <c r="N41" s="9" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6385,7 +6404,7 @@
         <v>709</v>
       </c>
       <c r="N42" s="9" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6427,7 +6446,7 @@
         <v>712</v>
       </c>
       <c r="N43" s="9" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6471,7 +6490,7 @@
         <v>720</v>
       </c>
       <c r="N44" s="9" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6511,7 +6530,7 @@
         <v>769</v>
       </c>
       <c r="N45" s="9" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6553,7 +6572,7 @@
         <v>717</v>
       </c>
       <c r="N46" s="9" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6595,7 +6614,7 @@
         <v>723</v>
       </c>
       <c r="N47" s="9" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6639,7 +6658,7 @@
         <v>729</v>
       </c>
       <c r="N48" s="9" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6683,7 +6702,7 @@
         <v>733</v>
       </c>
       <c r="N49" s="9" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6759,7 +6778,7 @@
         <v>640</v>
       </c>
       <c r="N51" s="9" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6801,7 +6820,7 @@
         <v>0</v>
       </c>
       <c r="N52" s="9" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6843,7 +6862,7 @@
         <v>643</v>
       </c>
       <c r="N53" s="9" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6879,7 +6898,7 @@
       <c r="L54" s="9"/>
       <c r="M54" s="9"/>
       <c r="N54" s="9" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6923,7 +6942,7 @@
         <v>645</v>
       </c>
       <c r="N55" s="9" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6967,7 +6986,7 @@
         <v>647</v>
       </c>
       <c r="N56" s="9" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="57" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7011,7 +7030,7 @@
         <v>650</v>
       </c>
       <c r="N57" s="9" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7053,7 +7072,7 @@
         <v>654</v>
       </c>
       <c r="N58" s="9" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="59" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7095,7 +7114,7 @@
         <v>656</v>
       </c>
       <c r="N59" s="9" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="60" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7131,7 +7150,7 @@
         <v>576</v>
       </c>
       <c r="N60" s="4" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7165,7 +7184,7 @@
         <v>776</v>
       </c>
       <c r="N61" s="9" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="62" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7207,7 +7226,7 @@
         <v>579</v>
       </c>
       <c r="N62" s="9" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="63" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7249,7 +7268,7 @@
         <v>582</v>
       </c>
       <c r="N63" s="9" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="64" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7291,7 +7310,7 @@
         <v>585</v>
       </c>
       <c r="N64" s="9" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7331,7 +7350,7 @@
         <v>779</v>
       </c>
       <c r="N65" s="9" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="66" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7375,7 +7394,7 @@
         <v>588</v>
       </c>
       <c r="N66" s="9" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="67" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7411,7 +7430,7 @@
       <c r="L67" s="9"/>
       <c r="M67" s="9"/>
       <c r="N67" s="9" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="68" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7455,7 +7474,7 @@
         <v>590</v>
       </c>
       <c r="N68" s="9" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="69" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7497,7 +7516,7 @@
         <v>592</v>
       </c>
       <c r="N69" s="9" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="70" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7541,7 +7560,7 @@
         <v>595</v>
       </c>
       <c r="N70" s="9" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="71" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7579,7 +7598,7 @@
         <v>540</v>
       </c>
       <c r="N71" s="9" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="72" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7621,7 +7640,7 @@
         <v>598</v>
       </c>
       <c r="N72" s="9" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="73" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7663,7 +7682,7 @@
         <v>600</v>
       </c>
       <c r="N73" s="9" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="74" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7699,7 +7718,7 @@
       <c r="L74" s="9"/>
       <c r="M74" s="9"/>
       <c r="N74" s="9" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="75" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7735,7 +7754,7 @@
       <c r="L75" s="9"/>
       <c r="M75" s="9"/>
       <c r="N75" s="9" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="76" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7771,7 +7790,7 @@
       <c r="L76" s="9"/>
       <c r="M76" s="9"/>
       <c r="N76" s="9" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="77" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7813,7 +7832,7 @@
         <v>602</v>
       </c>
       <c r="N77" s="9" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="78" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7853,7 +7872,7 @@
       <c r="L78" s="9"/>
       <c r="M78" s="9"/>
       <c r="N78" s="9" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="79" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7889,7 +7908,7 @@
       <c r="L79" s="9"/>
       <c r="M79" s="9"/>
       <c r="N79" s="9" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="80" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7963,7 +7982,7 @@
         <v>475</v>
       </c>
       <c r="N81" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="82" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7999,7 +8018,7 @@
         <v>520</v>
       </c>
       <c r="N82" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="83" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8043,7 +8062,7 @@
         <v>524</v>
       </c>
       <c r="N83" s="9" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="84" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8085,7 +8104,7 @@
         <v>532</v>
       </c>
       <c r="N84" s="9" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="85" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8127,7 +8146,7 @@
         <v>528</v>
       </c>
       <c r="N85" s="9" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="86" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8169,7 +8188,7 @@
         <v>535</v>
       </c>
       <c r="N86" s="9" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="87" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8245,7 +8264,7 @@
         <v>551</v>
       </c>
       <c r="N88" s="9" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="89" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8287,7 +8306,7 @@
         <v>548</v>
       </c>
       <c r="N89" s="9" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="90" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8331,7 +8350,7 @@
         <v>543</v>
       </c>
       <c r="N90" s="9" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="91" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8375,7 +8394,7 @@
         <v>546</v>
       </c>
       <c r="N91" s="9" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="92" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8413,7 +8432,7 @@
         <v>476</v>
       </c>
       <c r="N92" s="9" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="93" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8487,7 +8506,7 @@
         <v>684</v>
       </c>
       <c r="N94" s="9" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="95" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8529,7 +8548,7 @@
         <v>687</v>
       </c>
       <c r="N95" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="96" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8569,7 +8588,7 @@
         <v>754</v>
       </c>
       <c r="N96" s="9" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="97" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8639,7 +8658,7 @@
         <v>554</v>
       </c>
       <c r="N98" s="9" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="99" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8681,7 +8700,7 @@
         <v>558</v>
       </c>
       <c r="N99" s="9" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="100" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8713,7 +8732,7 @@
       </c>
       <c r="M100" s="4"/>
       <c r="N100" s="4" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="101" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8785,7 +8804,7 @@
         <v>507</v>
       </c>
       <c r="N102" s="9" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="103" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8827,7 +8846,7 @@
         <v>509</v>
       </c>
       <c r="N103" s="9" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="104" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8933,7 +8952,7 @@
         <v>485</v>
       </c>
       <c r="N106" s="9" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="107" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8975,7 +8994,7 @@
         <v>488</v>
       </c>
       <c r="N107" s="9" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="108" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9017,7 +9036,7 @@
         <v>479</v>
       </c>
       <c r="N108" s="9" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="109" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9059,7 +9078,7 @@
         <v>482</v>
       </c>
       <c r="N109" s="9" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="110" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9161,7 +9180,7 @@
         <v>470</v>
       </c>
       <c r="N112" s="9" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="113" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9227,7 +9246,7 @@
       <c r="L114" s="9"/>
       <c r="M114" s="9"/>
       <c r="N114" s="9" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="115" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9269,7 +9288,7 @@
         <v>512</v>
       </c>
       <c r="N115" s="9" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="116" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9311,7 +9330,7 @@
         <v>515</v>
       </c>
       <c r="N116" s="9" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="117" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9379,7 +9398,7 @@
         <v>755</v>
       </c>
       <c r="N118" s="9" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="119" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9419,7 +9438,7 @@
         <v>755</v>
       </c>
       <c r="N119" s="9" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="120" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9459,7 +9478,7 @@
         <v>757</v>
       </c>
       <c r="N120" s="9" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="121" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9529,7 +9548,7 @@
         <v>741</v>
       </c>
       <c r="N122" s="9" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="123" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9571,7 +9590,7 @@
         <v>738</v>
       </c>
       <c r="N123" s="9" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="124" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9613,7 +9632,7 @@
         <v>744</v>
       </c>
       <c r="N124" s="9" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="125" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9683,7 +9702,7 @@
         <v>746</v>
       </c>
       <c r="N126" s="9" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="127" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9723,7 +9742,7 @@
         <v>752</v>
       </c>
       <c r="N127" s="9" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="128" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9765,7 +9784,7 @@
         <v>748</v>
       </c>
       <c r="N128" s="9" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="129" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9807,7 +9826,7 @@
         <v>750</v>
       </c>
       <c r="N129" s="9" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="130" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9883,7 +9902,7 @@
         <v>668</v>
       </c>
       <c r="N131" s="9" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="132" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9925,7 +9944,7 @@
         <v>671</v>
       </c>
       <c r="N132" s="9" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="133" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9967,7 +9986,7 @@
         <v>674</v>
       </c>
       <c r="N133" s="9" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="134" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10009,7 +10028,7 @@
         <v>677</v>
       </c>
       <c r="N134" s="9" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="135" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10051,7 +10070,7 @@
         <v>680</v>
       </c>
       <c r="N135" s="9" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="136" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10121,7 +10140,7 @@
         <v>491</v>
       </c>
       <c r="N137" s="9" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="138" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10163,7 +10182,7 @@
         <v>493</v>
       </c>
       <c r="N138" s="9" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="139" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10205,7 +10224,7 @@
         <v>497</v>
       </c>
       <c r="N139" s="9" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="140" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10247,7 +10266,7 @@
         <v>495</v>
       </c>
       <c r="N140" s="9" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="141" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10289,7 +10308,7 @@
         <v>500</v>
       </c>
       <c r="N141" s="9" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="142" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10361,7 +10380,7 @@
         <v>468</v>
       </c>
       <c r="N143" s="9" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="144" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10433,7 +10452,7 @@
         <v>463</v>
       </c>
       <c r="N145" s="9" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="146" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10475,7 +10494,7 @@
         <v>465</v>
       </c>
       <c r="N146" s="9" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="147" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10551,7 +10570,7 @@
         <v>808</v>
       </c>
       <c r="N148" s="15" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="149" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10593,7 +10612,7 @@
         <v>809</v>
       </c>
       <c r="N149" s="15" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="150" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10635,7 +10654,7 @@
         <v>806</v>
       </c>
       <c r="N150" s="15" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="151" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10677,7 +10696,7 @@
         <v>817</v>
       </c>
       <c r="N151" s="18" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="152" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10719,7 +10738,7 @@
         <v>822</v>
       </c>
       <c r="N152" s="18" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="153" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10763,88 +10782,84 @@
         <v>823</v>
       </c>
       <c r="N153" s="18" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="154" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A154" s="17" t="s">
-        <v>831</v>
-      </c>
-      <c r="B154" s="25">
+        <v>830</v>
+      </c>
+      <c r="B154" s="23">
         <v>151</v>
       </c>
       <c r="C154" s="21" t="s">
+        <v>963</v>
+      </c>
+      <c r="D154" s="21" t="s">
         <v>826</v>
-      </c>
-      <c r="D154" s="21" t="s">
-        <v>827</v>
       </c>
       <c r="E154" s="21" t="s">
         <v>13</v>
       </c>
       <c r="F154" s="18" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="G154" s="14" t="s">
         <v>36</v>
       </c>
       <c r="H154" s="21" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="I154" s="21" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="J154" s="21" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="K154" s="21" t="s">
         <v>456</v>
       </c>
       <c r="L154" s="21" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="M154" s="21" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="N154" s="21" t="s">
-        <v>958</v>
-      </c>
-      <c r="O154" s="23"/>
-      <c r="P154" s="24"/>
-      <c r="Q154" s="24"/>
-      <c r="R154" s="24"/>
-      <c r="S154" s="24"/>
-      <c r="T154" s="23"/>
+        <v>957</v>
+      </c>
+      <c r="O154" s="20"/>
+      <c r="T154" s="20"/>
       <c r="U154" s="20"/>
       <c r="V154" s="22"/>
     </row>
     <row r="155" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A155" s="17" t="s">
-        <v>831</v>
-      </c>
-      <c r="B155" s="25">
+        <v>830</v>
+      </c>
+      <c r="B155" s="23">
         <v>152</v>
       </c>
       <c r="C155" s="21" t="s">
-        <v>826</v>
+        <v>963</v>
       </c>
       <c r="D155" s="21" t="s">
-        <v>960</v>
-      </c>
-      <c r="E155" s="26" t="s">
+        <v>959</v>
+      </c>
+      <c r="E155" s="24" t="s">
         <v>237</v>
       </c>
       <c r="F155" s="18" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="G155" s="14" t="s">
         <v>36</v>
       </c>
       <c r="H155" s="21" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="I155" s="21" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="J155" s="21" t="s">
         <v>611</v>
@@ -10853,13 +10868,57 @@
         <v>612</v>
       </c>
       <c r="L155" s="21" t="s">
-        <v>829</v>
+        <v>970</v>
       </c>
       <c r="M155" s="21" t="s">
-        <v>832</v>
+        <v>968</v>
       </c>
       <c r="N155" s="21" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="156" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A156" s="17" t="s">
+        <v>830</v>
+      </c>
+      <c r="B156" s="23">
+        <v>157</v>
+      </c>
+      <c r="C156" s="21" t="s">
         <v>963</v>
+      </c>
+      <c r="D156" s="21" t="s">
+        <v>964</v>
+      </c>
+      <c r="E156" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F156" s="18" t="s">
+        <v>965</v>
+      </c>
+      <c r="G156" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="H156" s="21" t="s">
+        <v>826</v>
+      </c>
+      <c r="I156" s="21" t="s">
+        <v>966</v>
+      </c>
+      <c r="J156" s="21" t="s">
+        <v>967</v>
+      </c>
+      <c r="K156" s="21" t="s">
+        <v>460</v>
+      </c>
+      <c r="L156" s="21" t="s">
+        <v>970</v>
+      </c>
+      <c r="M156" s="21" t="s">
+        <v>969</v>
+      </c>
+      <c r="N156" s="21" t="s">
+        <v>962</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added nc:ArrestIncident to Case Initiation and Charge Updates to carry Charge Item #
</commit_message>
<xml_diff>
--- a/schemas/CaseInitiation_iepd/artifacts/CaseInitiation_MappingSpreasheet.xlsx
+++ b/schemas/CaseInitiation_iepd/artifacts/CaseInitiation_MappingSpreasheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\CaseInitiation_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A054E6F-5E32-4215-B081-C4185188196A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684349BB-4ECA-4761-915E-D5E8BF4EFAB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4080" yWindow="-21720" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Case Initiation" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="971">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1845" uniqueCount="977">
   <si>
     <t/>
   </si>
@@ -3096,9 +3096,6 @@
     <t>nola-ext:ChargeDispositionCode</t>
   </si>
   <si>
-    <t>Charge Disposition Code</t>
-  </si>
-  <si>
     <t>j:CaseCharge/nola-ext:ChargeAugmentation/nola-ext:ChargeDispositionCode</t>
   </si>
   <si>
@@ -3554,6 +3551,28 @@
   </si>
   <si>
     <t>nc:DispositionType</t>
+  </si>
+  <si>
+    <t>Charge Item Number</t>
+  </si>
+  <si>
+    <t>An identification that references an activity.
+The Item # is the incident number assigned by the Computer Aided Dispatching. It will be included on all arrest paperwork submitted by the arresting officer.</t>
+  </si>
+  <si>
+    <t>nc:ActivityIdentification</t>
+  </si>
+  <si>
+    <t>nc:ActivityType</t>
+  </si>
+  <si>
+    <t>/j:Arrest/j:ArrestCharge/nola-ext:ChargeAugmentation/nola-ext:ArrestIncident/nc:ActivityIdentification/nc:IndentificationID</t>
+  </si>
+  <si>
+    <t>nola:CaseInitiationExchange/j:Arrest/j:ArrestCharge/nola-ext:ChargeAugmentation/nola-ext:ArrestIncident/nc:ActivityIdentification/nc:IndentificationID</t>
+  </si>
+  <si>
+    <t>ChargeItemNumber</t>
   </si>
 </sst>
 </file>
@@ -3625,7 +3644,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -3727,20 +3746,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3803,15 +3813,25 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4719,13 +4739,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V156"/>
+  <dimension ref="A1:P158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E137" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E131" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N156" sqref="A154:N156"/>
+      <selection pane="bottomRight" activeCell="F165" sqref="F165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -4737,6 +4757,7 @@
     <col min="5" max="5" width="30.1328125" customWidth="1"/>
     <col min="6" max="6" width="35.6640625" customWidth="1"/>
     <col min="7" max="7" width="13.19921875" customWidth="1"/>
+    <col min="8" max="8" width="31.73046875" customWidth="1"/>
     <col min="9" max="9" width="126.33203125" customWidth="1"/>
     <col min="10" max="12" width="11" customWidth="1"/>
     <col min="13" max="13" width="15.1328125" customWidth="1"/>
@@ -4854,7 +4875,7 @@
         <v>561</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -4896,7 +4917,7 @@
         <v>563</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -4938,7 +4959,7 @@
         <v>566</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -4980,7 +5001,7 @@
         <v>570</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5022,7 +5043,7 @@
         <v>573</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5094,7 +5115,7 @@
         <v>461</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5136,7 +5157,7 @@
         <v>457</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5208,7 +5229,7 @@
         <v>504</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5238,7 +5259,7 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5280,7 +5301,7 @@
         <v>606</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5322,7 +5343,7 @@
         <v>609</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5364,7 +5385,7 @@
         <v>613</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5406,7 +5427,7 @@
         <v>615</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5448,7 +5469,7 @@
         <v>617</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5490,7 +5511,7 @@
         <v>620</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5532,7 +5553,7 @@
         <v>623</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5574,7 +5595,7 @@
         <v>626</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5616,7 +5637,7 @@
         <v>629</v>
       </c>
       <c r="N22" s="9" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5658,7 +5679,7 @@
         <v>632</v>
       </c>
       <c r="N23" s="9" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5722,7 +5743,7 @@
         <v>773</v>
       </c>
       <c r="N25" s="9" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5764,7 +5785,7 @@
         <v>659</v>
       </c>
       <c r="N26" s="9" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5806,7 +5827,7 @@
         <v>661</v>
       </c>
       <c r="N27" s="9" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5904,7 +5925,7 @@
         <v>693</v>
       </c>
       <c r="N30" s="9" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5946,7 +5967,7 @@
         <v>0</v>
       </c>
       <c r="N31" s="9" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5984,7 +6005,7 @@
         <v>760</v>
       </c>
       <c r="N32" s="9" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6024,7 +6045,7 @@
         <v>764</v>
       </c>
       <c r="N33" s="9" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6066,7 +6087,7 @@
         <v>715</v>
       </c>
       <c r="N34" s="9" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6106,7 +6127,7 @@
       <c r="L35" s="9"/>
       <c r="M35" s="9"/>
       <c r="N35" s="9" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6148,7 +6169,7 @@
         <v>697</v>
       </c>
       <c r="N36" s="9" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6192,7 +6213,7 @@
         <v>699</v>
       </c>
       <c r="N37" s="9" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6236,7 +6257,7 @@
         <v>807</v>
       </c>
       <c r="N38" s="9" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6278,7 +6299,7 @@
         <v>726</v>
       </c>
       <c r="N39" s="9" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6320,7 +6341,7 @@
         <v>703</v>
       </c>
       <c r="N40" s="9" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6362,7 +6383,7 @@
         <v>706</v>
       </c>
       <c r="N41" s="9" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6404,7 +6425,7 @@
         <v>709</v>
       </c>
       <c r="N42" s="9" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6446,7 +6467,7 @@
         <v>712</v>
       </c>
       <c r="N43" s="9" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6490,7 +6511,7 @@
         <v>720</v>
       </c>
       <c r="N44" s="9" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6530,7 +6551,7 @@
         <v>769</v>
       </c>
       <c r="N45" s="9" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6572,7 +6593,7 @@
         <v>717</v>
       </c>
       <c r="N46" s="9" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6614,7 +6635,7 @@
         <v>723</v>
       </c>
       <c r="N47" s="9" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6658,7 +6679,7 @@
         <v>729</v>
       </c>
       <c r="N48" s="9" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6702,7 +6723,7 @@
         <v>733</v>
       </c>
       <c r="N49" s="9" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6778,7 +6799,7 @@
         <v>640</v>
       </c>
       <c r="N51" s="9" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6820,7 +6841,7 @@
         <v>0</v>
       </c>
       <c r="N52" s="9" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6862,7 +6883,7 @@
         <v>643</v>
       </c>
       <c r="N53" s="9" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6898,7 +6919,7 @@
       <c r="L54" s="9"/>
       <c r="M54" s="9"/>
       <c r="N54" s="9" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6942,7 +6963,7 @@
         <v>645</v>
       </c>
       <c r="N55" s="9" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6986,7 +7007,7 @@
         <v>647</v>
       </c>
       <c r="N56" s="9" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="57" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7030,7 +7051,7 @@
         <v>650</v>
       </c>
       <c r="N57" s="9" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7072,7 +7093,7 @@
         <v>654</v>
       </c>
       <c r="N58" s="9" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="59" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7114,7 +7135,7 @@
         <v>656</v>
       </c>
       <c r="N59" s="9" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="60" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7150,7 +7171,7 @@
         <v>576</v>
       </c>
       <c r="N60" s="4" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7184,7 +7205,7 @@
         <v>776</v>
       </c>
       <c r="N61" s="9" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="62" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7226,7 +7247,7 @@
         <v>579</v>
       </c>
       <c r="N62" s="9" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="63" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7268,7 +7289,7 @@
         <v>582</v>
       </c>
       <c r="N63" s="9" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="64" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7310,7 +7331,7 @@
         <v>585</v>
       </c>
       <c r="N64" s="9" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7350,7 +7371,7 @@
         <v>779</v>
       </c>
       <c r="N65" s="9" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="66" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7394,7 +7415,7 @@
         <v>588</v>
       </c>
       <c r="N66" s="9" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="67" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7430,7 +7451,7 @@
       <c r="L67" s="9"/>
       <c r="M67" s="9"/>
       <c r="N67" s="9" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="68" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7474,7 +7495,7 @@
         <v>590</v>
       </c>
       <c r="N68" s="9" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="69" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7516,7 +7537,7 @@
         <v>592</v>
       </c>
       <c r="N69" s="9" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="70" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7560,7 +7581,7 @@
         <v>595</v>
       </c>
       <c r="N70" s="9" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="71" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7598,7 +7619,7 @@
         <v>540</v>
       </c>
       <c r="N71" s="9" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="72" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7640,7 +7661,7 @@
         <v>598</v>
       </c>
       <c r="N72" s="9" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="73" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7682,7 +7703,7 @@
         <v>600</v>
       </c>
       <c r="N73" s="9" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="74" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7718,7 +7739,7 @@
       <c r="L74" s="9"/>
       <c r="M74" s="9"/>
       <c r="N74" s="9" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="75" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7754,7 +7775,7 @@
       <c r="L75" s="9"/>
       <c r="M75" s="9"/>
       <c r="N75" s="9" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="76" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7790,7 +7811,7 @@
       <c r="L76" s="9"/>
       <c r="M76" s="9"/>
       <c r="N76" s="9" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="77" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7832,7 +7853,7 @@
         <v>602</v>
       </c>
       <c r="N77" s="9" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="78" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7872,7 +7893,7 @@
       <c r="L78" s="9"/>
       <c r="M78" s="9"/>
       <c r="N78" s="9" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="79" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7908,7 +7929,7 @@
       <c r="L79" s="9"/>
       <c r="M79" s="9"/>
       <c r="N79" s="9" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="80" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7982,7 +8003,7 @@
         <v>475</v>
       </c>
       <c r="N81" s="9" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="82" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8018,7 +8039,7 @@
         <v>520</v>
       </c>
       <c r="N82" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="83" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8062,7 +8083,7 @@
         <v>524</v>
       </c>
       <c r="N83" s="9" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="84" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8104,7 +8125,7 @@
         <v>532</v>
       </c>
       <c r="N84" s="9" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="85" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8146,7 +8167,7 @@
         <v>528</v>
       </c>
       <c r="N85" s="9" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="86" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8188,7 +8209,7 @@
         <v>535</v>
       </c>
       <c r="N86" s="9" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="87" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8264,7 +8285,7 @@
         <v>551</v>
       </c>
       <c r="N88" s="9" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="89" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8306,7 +8327,7 @@
         <v>548</v>
       </c>
       <c r="N89" s="9" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="90" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8350,7 +8371,7 @@
         <v>543</v>
       </c>
       <c r="N90" s="9" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="91" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8394,7 +8415,7 @@
         <v>546</v>
       </c>
       <c r="N91" s="9" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="92" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8432,7 +8453,7 @@
         <v>476</v>
       </c>
       <c r="N92" s="9" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="93" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8506,7 +8527,7 @@
         <v>684</v>
       </c>
       <c r="N94" s="9" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="95" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8548,7 +8569,7 @@
         <v>687</v>
       </c>
       <c r="N95" s="9" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="96" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8588,7 +8609,7 @@
         <v>754</v>
       </c>
       <c r="N96" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="97" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8658,7 +8679,7 @@
         <v>554</v>
       </c>
       <c r="N98" s="9" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="99" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8700,7 +8721,7 @@
         <v>558</v>
       </c>
       <c r="N99" s="9" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="100" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8732,7 +8753,7 @@
       </c>
       <c r="M100" s="4"/>
       <c r="N100" s="4" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="101" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8804,7 +8825,7 @@
         <v>507</v>
       </c>
       <c r="N102" s="9" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="103" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8846,7 +8867,7 @@
         <v>509</v>
       </c>
       <c r="N103" s="9" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="104" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8952,7 +8973,7 @@
         <v>485</v>
       </c>
       <c r="N106" s="9" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="107" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8994,7 +9015,7 @@
         <v>488</v>
       </c>
       <c r="N107" s="9" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="108" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9036,7 +9057,7 @@
         <v>479</v>
       </c>
       <c r="N108" s="9" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="109" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9078,7 +9099,7 @@
         <v>482</v>
       </c>
       <c r="N109" s="9" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="110" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9180,7 +9201,7 @@
         <v>470</v>
       </c>
       <c r="N112" s="9" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="113" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9246,7 +9267,7 @@
       <c r="L114" s="9"/>
       <c r="M114" s="9"/>
       <c r="N114" s="9" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="115" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9288,7 +9309,7 @@
         <v>512</v>
       </c>
       <c r="N115" s="9" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="116" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9330,7 +9351,7 @@
         <v>515</v>
       </c>
       <c r="N116" s="9" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="117" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9398,7 +9419,7 @@
         <v>755</v>
       </c>
       <c r="N118" s="9" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="119" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9438,7 +9459,7 @@
         <v>755</v>
       </c>
       <c r="N119" s="9" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="120" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9478,7 +9499,7 @@
         <v>757</v>
       </c>
       <c r="N120" s="9" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="121" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9548,7 +9569,7 @@
         <v>741</v>
       </c>
       <c r="N122" s="9" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="123" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9590,7 +9611,7 @@
         <v>738</v>
       </c>
       <c r="N123" s="9" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="124" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9632,7 +9653,7 @@
         <v>744</v>
       </c>
       <c r="N124" s="9" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="125" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9702,7 +9723,7 @@
         <v>746</v>
       </c>
       <c r="N126" s="9" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="127" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9742,7 +9763,7 @@
         <v>752</v>
       </c>
       <c r="N127" s="9" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="128" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9784,7 +9805,7 @@
         <v>748</v>
       </c>
       <c r="N128" s="9" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="129" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9826,7 +9847,7 @@
         <v>750</v>
       </c>
       <c r="N129" s="9" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="130" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9902,7 +9923,7 @@
         <v>668</v>
       </c>
       <c r="N131" s="9" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="132" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9944,7 +9965,7 @@
         <v>671</v>
       </c>
       <c r="N132" s="9" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="133" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9986,7 +10007,7 @@
         <v>674</v>
       </c>
       <c r="N133" s="9" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="134" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10028,7 +10049,7 @@
         <v>677</v>
       </c>
       <c r="N134" s="9" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="135" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10070,7 +10091,7 @@
         <v>680</v>
       </c>
       <c r="N135" s="9" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="136" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10140,7 +10161,7 @@
         <v>491</v>
       </c>
       <c r="N137" s="9" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="138" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10182,7 +10203,7 @@
         <v>493</v>
       </c>
       <c r="N138" s="9" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="139" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10224,7 +10245,7 @@
         <v>497</v>
       </c>
       <c r="N139" s="9" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="140" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10266,7 +10287,7 @@
         <v>495</v>
       </c>
       <c r="N140" s="9" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="141" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10308,7 +10329,7 @@
         <v>500</v>
       </c>
       <c r="N141" s="9" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="142" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10380,7 +10401,7 @@
         <v>468</v>
       </c>
       <c r="N143" s="9" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="144" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10413,7 +10434,7 @@
       <c r="M144" s="4"/>
       <c r="N144" s="4"/>
     </row>
-    <row r="145" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A145" s="7" t="s">
         <v>12</v>
       </c>
@@ -10452,10 +10473,10 @@
         <v>463</v>
       </c>
       <c r="N145" s="9" t="s">
-        <v>949</v>
-      </c>
-    </row>
-    <row r="146" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="146" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A146" s="7" t="s">
         <v>12</v>
       </c>
@@ -10494,10 +10515,10 @@
         <v>465</v>
       </c>
       <c r="N146" s="9" t="s">
-        <v>950</v>
-      </c>
-    </row>
-    <row r="147" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="147" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A147" s="12" t="s">
         <v>12</v>
       </c>
@@ -10531,7 +10552,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="148" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A148" s="12" t="s">
         <v>12</v>
       </c>
@@ -10570,10 +10591,10 @@
         <v>808</v>
       </c>
       <c r="N148" s="15" t="s">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="149" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="149" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A149" s="12" t="s">
         <v>12</v>
       </c>
@@ -10612,10 +10633,10 @@
         <v>809</v>
       </c>
       <c r="N149" s="15" t="s">
-        <v>952</v>
-      </c>
-    </row>
-    <row r="150" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="150" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A150" s="12" t="s">
         <v>12</v>
       </c>
@@ -10654,10 +10675,10 @@
         <v>806</v>
       </c>
       <c r="N150" s="15" t="s">
-        <v>953</v>
-      </c>
-    </row>
-    <row r="151" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="151" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A151" s="17" t="s">
         <v>12</v>
       </c>
@@ -10696,10 +10717,10 @@
         <v>817</v>
       </c>
       <c r="N151" s="18" t="s">
-        <v>954</v>
-      </c>
-    </row>
-    <row r="152" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="152" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A152" s="17" t="s">
         <v>12</v>
       </c>
@@ -10738,10 +10759,10 @@
         <v>822</v>
       </c>
       <c r="N152" s="18" t="s">
-        <v>955</v>
-      </c>
-    </row>
-    <row r="153" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="153" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A153" s="17" t="s">
         <v>12</v>
       </c>
@@ -10782,18 +10803,18 @@
         <v>823</v>
       </c>
       <c r="N153" s="18" t="s">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="154" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="154" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A154" s="17" t="s">
-        <v>830</v>
-      </c>
-      <c r="B154" s="23">
+        <v>12</v>
+      </c>
+      <c r="B154" s="22">
         <v>151</v>
       </c>
       <c r="C154" s="21" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="D154" s="21" t="s">
         <v>826</v>
@@ -10811,7 +10832,7 @@
         <v>826</v>
       </c>
       <c r="I154" s="21" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="J154" s="21" t="s">
         <v>829</v>
@@ -10823,34 +10844,31 @@
         <v>828</v>
       </c>
       <c r="M154" s="21" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="N154" s="21" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="O154" s="20"/>
-      <c r="T154" s="20"/>
-      <c r="U154" s="20"/>
-      <c r="V154" s="22"/>
-    </row>
-    <row r="155" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="155" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A155" s="17" t="s">
-        <v>830</v>
-      </c>
-      <c r="B155" s="23">
+        <v>12</v>
+      </c>
+      <c r="B155" s="22">
         <v>152</v>
       </c>
       <c r="C155" s="21" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="D155" s="21" t="s">
-        <v>959</v>
-      </c>
-      <c r="E155" s="24" t="s">
+        <v>958</v>
+      </c>
+      <c r="E155" s="23" t="s">
         <v>237</v>
       </c>
       <c r="F155" s="18" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G155" s="14" t="s">
         <v>36</v>
@@ -10859,7 +10877,7 @@
         <v>826</v>
       </c>
       <c r="I155" s="21" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="J155" s="21" t="s">
         <v>611</v>
@@ -10868,33 +10886,33 @@
         <v>612</v>
       </c>
       <c r="L155" s="21" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="M155" s="21" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="N155" s="21" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="156" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A156" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B156" s="22">
+        <v>157</v>
+      </c>
+      <c r="C156" s="21" t="s">
         <v>962</v>
       </c>
-    </row>
-    <row r="156" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A156" s="17" t="s">
-        <v>830</v>
-      </c>
-      <c r="B156" s="23">
-        <v>157</v>
-      </c>
-      <c r="C156" s="21" t="s">
+      <c r="D156" s="21" t="s">
         <v>963</v>
       </c>
-      <c r="D156" s="21" t="s">
+      <c r="E156" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F156" s="18" t="s">
         <v>964</v>
-      </c>
-      <c r="E156" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="F156" s="18" t="s">
-        <v>965</v>
       </c>
       <c r="G156" s="14" t="s">
         <v>36</v>
@@ -10903,23 +10921,69 @@
         <v>826</v>
       </c>
       <c r="I156" s="21" t="s">
+        <v>965</v>
+      </c>
+      <c r="J156" s="21" t="s">
         <v>966</v>
-      </c>
-      <c r="J156" s="21" t="s">
-        <v>967</v>
       </c>
       <c r="K156" s="21" t="s">
         <v>460</v>
       </c>
       <c r="L156" s="21" t="s">
+        <v>969</v>
+      </c>
+      <c r="M156" s="21" t="s">
+        <v>968</v>
+      </c>
+      <c r="N156" s="21" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="157" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A157" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B157" s="16"/>
+      <c r="C157" s="19" t="s">
+        <v>328</v>
+      </c>
+      <c r="D157" s="22" t="s">
         <v>970</v>
       </c>
-      <c r="M156" s="21" t="s">
-        <v>969</v>
-      </c>
-      <c r="N156" s="21" t="s">
-        <v>962</v>
-      </c>
+      <c r="E157" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F157" s="27" t="s">
+        <v>971</v>
+      </c>
+      <c r="G157" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="H157" s="16" t="s">
+        <v>976</v>
+      </c>
+      <c r="I157" s="27"/>
+      <c r="J157" s="16" t="s">
+        <v>972</v>
+      </c>
+      <c r="K157" s="16" t="s">
+        <v>805</v>
+      </c>
+      <c r="L157" s="16" t="s">
+        <v>973</v>
+      </c>
+      <c r="M157" s="28" t="s">
+        <v>974</v>
+      </c>
+      <c r="N157" s="28" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="158" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A158" s="25"/>
+      <c r="B158" s="25"/>
+      <c r="O158" s="26"/>
+      <c r="P158" s="26"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O147">
@@ -10927,6 +10991,11 @@
     <sortCondition ref="D2:D147"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I157" xr:uid="{AFB63C6F-EC77-446D-B4A9-E737585DDD05}">
+      <formula1>MAPPING_CODES</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Added nola-ext:CourtCaseFollowCaseIdentification for CourtCaseFollowsCaseID in CaseInitation and ChargeUpdate
</commit_message>
<xml_diff>
--- a/schemas/CaseInitiation_iepd/artifacts/CaseInitiation_MappingSpreasheet.xlsx
+++ b/schemas/CaseInitiation_iepd/artifacts/CaseInitiation_MappingSpreasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\CaseInitiation_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684349BB-4ECA-4761-915E-D5E8BF4EFAB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76AE029F-FA91-48C7-AA2C-CDC416D5909A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4080" yWindow="-21720" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Case Initiation" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1845" uniqueCount="977">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1857" uniqueCount="982">
   <si>
     <t/>
   </si>
@@ -3556,23 +3556,38 @@
     <t>Charge Item Number</t>
   </si>
   <si>
+    <t>nc:ActivityIdentification</t>
+  </si>
+  <si>
+    <t>nc:ActivityType</t>
+  </si>
+  <si>
+    <t>/j:Arrest/j:ArrestCharge/nola-ext:ChargeAugmentation/nola-ext:ArrestIncident/nc:ActivityIdentification/nc:IndentificationID</t>
+  </si>
+  <si>
+    <t>nola:CaseInitiationExchange/j:Arrest/j:ArrestCharge/nola-ext:ChargeAugmentation/nola-ext:ArrestIncident/nc:ActivityIdentification/nc:IndentificationID</t>
+  </si>
+  <si>
+    <t>ChargeItemNumber</t>
+  </si>
+  <si>
+    <t>CourtCaseFollowCaseID</t>
+  </si>
+  <si>
+    <t>Identifies an existing court case that this case should follow</t>
+  </si>
+  <si>
+    <t>/nc:CourtCase/nola-ext:CaseAugmentation/nola-ext:CourtCaseFollowCaseIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/nc:CaseInitiationExchange/nc:CourtCase/nola-ext:CaseAugmentation/nola-ext:CourtCaseFollowCaseIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>nola-ext:CourtCaseFollowCaseIdentification</t>
+  </si>
+  <si>
     <t>An identification that references an activity.
 The Item # is the incident number assigned by the Computer Aided Dispatching. It will be included on all arrest paperwork submitted by the arresting officer.</t>
-  </si>
-  <si>
-    <t>nc:ActivityIdentification</t>
-  </si>
-  <si>
-    <t>nc:ActivityType</t>
-  </si>
-  <si>
-    <t>/j:Arrest/j:ArrestCharge/nola-ext:ChargeAugmentation/nola-ext:ArrestIncident/nc:ActivityIdentification/nc:IndentificationID</t>
-  </si>
-  <si>
-    <t>nola:CaseInitiationExchange/j:Arrest/j:ArrestCharge/nola-ext:ChargeAugmentation/nola-ext:ArrestIncident/nc:ActivityIdentification/nc:IndentificationID</t>
-  </si>
-  <si>
-    <t>ChargeItemNumber</t>
   </si>
 </sst>
 </file>
@@ -3750,7 +3765,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3819,11 +3834,8 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -4742,10 +4754,10 @@
   <dimension ref="A1:P158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E131" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="N131" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F165" sqref="F165"/>
+      <selection pane="bottomRight" activeCell="N157" sqref="N157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -10950,40 +10962,76 @@
       <c r="D157" s="22" t="s">
         <v>970</v>
       </c>
-      <c r="E157" s="27" t="s">
+      <c r="E157" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="F157" s="27" t="s">
+      <c r="F157" s="26" t="s">
+        <v>981</v>
+      </c>
+      <c r="G157" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="H157" s="16" t="s">
+        <v>975</v>
+      </c>
+      <c r="I157" s="26"/>
+      <c r="J157" s="16" t="s">
         <v>971</v>
-      </c>
-      <c r="G157" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="H157" s="16" t="s">
-        <v>976</v>
-      </c>
-      <c r="I157" s="27"/>
-      <c r="J157" s="16" t="s">
-        <v>972</v>
       </c>
       <c r="K157" s="16" t="s">
         <v>805</v>
       </c>
       <c r="L157" s="16" t="s">
+        <v>972</v>
+      </c>
+      <c r="M157" s="27" t="s">
         <v>973</v>
       </c>
-      <c r="M157" s="28" t="s">
+      <c r="N157" s="27" t="s">
         <v>974</v>
       </c>
-      <c r="N157" s="28" t="s">
-        <v>975</v>
-      </c>
     </row>
     <row r="158" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A158" s="25"/>
-      <c r="B158" s="25"/>
-      <c r="O158" s="26"/>
-      <c r="P158" s="26"/>
+      <c r="A158" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B158" s="19"/>
+      <c r="C158" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="D158" s="21" t="s">
+        <v>976</v>
+      </c>
+      <c r="E158" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F158" s="16" t="s">
+        <v>977</v>
+      </c>
+      <c r="G158" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H158" s="21" t="s">
+        <v>976</v>
+      </c>
+      <c r="I158" s="16"/>
+      <c r="J158" s="16" t="s">
+        <v>980</v>
+      </c>
+      <c r="K158" s="16" t="s">
+        <v>805</v>
+      </c>
+      <c r="L158" s="16" t="s">
+        <v>828</v>
+      </c>
+      <c r="M158" s="27" t="s">
+        <v>978</v>
+      </c>
+      <c r="N158" s="27" t="s">
+        <v>979</v>
+      </c>
+      <c r="O158" s="25"/>
+      <c r="P158" s="25"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O147">

</xml_diff>